<commit_message>
Combat, Colision, Movement, Keys, Doors, Levers, all working. needs more code, tho. Needs Health Potions and Weapons
</commit_message>
<xml_diff>
--- a/template mapas.xlsx
+++ b/template mapas.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1585955463" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1585955463" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1585955463" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1585955463"/>
+      <pm:revision xmlns:pm="smNativeData" day="1585986283" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1585986283" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1585986283" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1585986283"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
   <si>
     <t>x</t>
   </si>
@@ -37,7 +37,7 @@
     <t>D</t>
   </si>
   <si>
-    <t>|</t>
+    <t>#</t>
   </si>
   <si>
     <t>E</t>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>\</t>
+  </si>
+  <si>
+    <t>|</t>
   </si>
   <si>
     <t>_</t>
@@ -125,7 +128,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1585955463" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1585986283" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -141,7 +144,7 @@
       <sz val="20"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1585955463" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1585986283" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="400" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -157,7 +160,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1585955463" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1585986283" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -166,7 +169,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,7 +182,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585955463" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -190,7 +193,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585955463" type="1" fgLvl="71" fgClr="00FFFFFF" bgLvl="29" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="71" fgClr="00FFFFFF" bgLvl="29" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -201,7 +204,73 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585955463" type="1" fgLvl="0" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="0" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4D4D4D"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="100" fgClr="004D4D4D" bgLvl="0" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB3B3B3"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="100" fgClr="00B3B3B3" bgLvl="0" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7F7F7F"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="100" fgClr="007F7F7F" bgLvl="0" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="100" fgClr="00000000" bgLvl="0" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE6E6E6"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -212,101 +281,13 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585955463" type="1" fgLvl="100" fgClr="00333333" bgLvl="0" bgClr="00FFFFFF"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4D4D4D"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585955463" type="1" fgLvl="100" fgClr="004D4D4D" bgLvl="0" bgClr="00FFFFFF"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFB3B3B3"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585955463" type="1" fgLvl="100" fgClr="00B3B3B3" bgLvl="0" bgClr="00FFFFFF"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7F7F7F"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585955463" type="1" fgLvl="100" fgClr="007F7F7F" bgLvl="0" bgClr="00FFFFFF"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585955463" type="1" fgLvl="100" fgClr="00000000" bgLvl="0" bgClr="00FFFFFF"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585955463" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE6E6E6"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585955463" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF666666"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585955463" type="1" fgLvl="100" fgClr="00666666" bgLvl="0" bgClr="00FFFFFF"/>
-          </ext>
-        </extLst>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF999999"/>
-        <bgColor rgb="FFFFFFFF"/>
-        <extLst>
-          <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585955463" type="1" fgLvl="100" fgClr="00999999" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="100" fgClr="00333333" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="11">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -322,7 +303,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585955463"/>
+          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
         </ext>
       </extLst>
     </border>
@@ -341,7 +322,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585955463"/>
+          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
         </ext>
       </extLst>
     </border>
@@ -360,7 +341,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585955463"/>
+          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
         </ext>
       </extLst>
     </border>
@@ -379,7 +360,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585955463"/>
+          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
         </ext>
       </extLst>
     </border>
@@ -398,7 +379,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585955463"/>
+          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
         </ext>
       </extLst>
     </border>
@@ -417,7 +398,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585955463"/>
+          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
         </ext>
       </extLst>
     </border>
@@ -436,7 +417,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585955463"/>
+          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
         </ext>
       </extLst>
     </border>
@@ -455,7 +436,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585955463"/>
+          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
         </ext>
       </extLst>
     </border>
@@ -474,7 +455,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585955463"/>
+          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
         </ext>
       </extLst>
     </border>
@@ -493,7 +474,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585955463"/>
+          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
         </ext>
       </extLst>
     </border>
@@ -512,45 +493,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585955463"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585955463"/>
-        </ext>
-      </extLst>
-    </border>
-    <border>
-      <left style="none">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="none">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="none">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="none">
-        <color rgb="FF000000"/>
-      </bottom>
-      <extLst>
-        <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585955463"/>
+          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
         </ext>
       </extLst>
     </border>
@@ -558,7 +501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -575,7 +518,46 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -584,48 +566,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -633,10 +573,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1585955463" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1585986283" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1585955463" count="4">
+      <pm:colors xmlns:pm="smNativeData" id="1585986283" count="4">
         <pm:color name="Cor 24" rgb="FFFF9E"/>
         <pm:color name="Cor 25" rgb="B5B5B5"/>
         <pm:color name="Cor 26" rgb="6B6B6B"/>
@@ -905,14 +845,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CZ65"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" zoomScale="60" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="AC1" zoomScale="60" workbookViewId="0">
+      <selection activeCell="AU18" sqref="AU18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="24.95"/>
   <cols>
     <col min="1" max="1" width="10.000000" style="1"/>
-    <col min="2" max="104" width="3.828829" customWidth="1" style="2"/>
+    <col min="2" max="63" width="3.828829" customWidth="1" style="2"/>
+    <col min="64" max="64" width="4.810811" customWidth="1" style="2"/>
+    <col min="65" max="104" width="3.828829" customWidth="1" style="2"/>
     <col min="105" max="16384" width="10.000000" style="2"/>
   </cols>
   <sheetData>
@@ -1168,7 +1110,7 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
+      <c r="Q2" s="21"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
@@ -1193,8 +1135,8 @@
       <c r="AM2" s="5"/>
       <c r="AN2" s="5"/>
       <c r="AO2" s="5"/>
-      <c r="AP2" s="14"/>
-      <c r="AQ2" s="14"/>
+      <c r="AP2" s="10"/>
+      <c r="AQ2" s="10"/>
       <c r="AR2" s="10"/>
       <c r="AS2" s="10"/>
       <c r="AT2" s="10"/>
@@ -1217,7 +1159,9 @@
       <c r="BK2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL2" s="12"/>
+      <c r="BL2" s="12" t="n">
+        <v>0</v>
+      </c>
       <c r="BM2" s="12"/>
       <c r="BN2" s="12"/>
       <c r="BO2" s="12"/>
@@ -1266,8 +1210,8 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="8"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="6"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
       <c r="K3" s="8"/>
@@ -1276,8 +1220,8 @@
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="8"/>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="6"/>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
       <c r="U3" s="8"/>
@@ -1301,8 +1245,8 @@
       <c r="AM3" s="8"/>
       <c r="AN3" s="8"/>
       <c r="AO3" s="6"/>
-      <c r="AP3" s="16"/>
-      <c r="AQ3" s="16"/>
+      <c r="AP3" s="8"/>
+      <c r="AQ3" s="8"/>
       <c r="AR3" s="8"/>
       <c r="AS3" s="8"/>
       <c r="AT3" s="8"/>
@@ -1325,7 +1269,9 @@
       <c r="BK3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL3" s="12"/>
+      <c r="BL3" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="BM3" s="12"/>
       <c r="BN3" s="12"/>
       <c r="BO3" s="12"/>
@@ -1374,8 +1320,8 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
@@ -1384,8 +1330,8 @@
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="7"/>
+      <c r="Q4" s="18"/>
+      <c r="R4" s="8"/>
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
@@ -1411,8 +1357,8 @@
         <v>1</v>
       </c>
       <c r="AO4" s="6"/>
-      <c r="AP4" s="15"/>
-      <c r="AQ4" s="15"/>
+      <c r="AP4" s="7"/>
+      <c r="AQ4" s="7"/>
       <c r="AR4" s="7"/>
       <c r="AS4" s="7"/>
       <c r="AT4" s="7"/>
@@ -1439,7 +1385,9 @@
       <c r="BK4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL4" s="12"/>
+      <c r="BL4" s="12" t="n">
+        <v>2</v>
+      </c>
       <c r="BM4" s="12"/>
       <c r="BN4" s="12"/>
       <c r="BO4" s="12"/>
@@ -1490,10 +1438,10 @@
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="18"/>
+      <c r="H5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
@@ -1502,10 +1450,10 @@
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
-      <c r="Q5" s="7" t="s">
+      <c r="Q5" s="18"/>
+      <c r="R5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
       <c r="U5" s="7"/>
@@ -1529,8 +1477,8 @@
       <c r="AM5" s="7"/>
       <c r="AN5" s="7"/>
       <c r="AO5" s="6"/>
-      <c r="AP5" s="15"/>
-      <c r="AQ5" s="15"/>
+      <c r="AP5" s="7"/>
+      <c r="AQ5" s="7"/>
       <c r="AR5" s="7"/>
       <c r="AS5" s="7"/>
       <c r="AT5" s="6"/>
@@ -1553,7 +1501,9 @@
       <c r="BK5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL5" s="12"/>
+      <c r="BL5" s="12" t="n">
+        <v>3</v>
+      </c>
       <c r="BM5" s="12"/>
       <c r="BN5" s="12"/>
       <c r="BO5" s="12"/>
@@ -1602,8 +1552,8 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="6"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
@@ -1612,8 +1562,8 @@
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="7"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="6"/>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
       <c r="U6" s="7"/>
@@ -1637,8 +1587,8 @@
       <c r="AM6" s="7"/>
       <c r="AN6" s="7"/>
       <c r="AO6" s="6"/>
-      <c r="AP6" s="15"/>
-      <c r="AQ6" s="15"/>
+      <c r="AP6" s="7"/>
+      <c r="AQ6" s="7"/>
       <c r="AR6" s="7"/>
       <c r="AS6" s="7"/>
       <c r="AT6" s="6"/>
@@ -1649,7 +1599,9 @@
       <c r="AY6" s="6"/>
       <c r="AZ6" s="7"/>
       <c r="BA6" s="7"/>
-      <c r="BB6" s="7"/>
+      <c r="BB6" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="BC6" s="7"/>
       <c r="BD6" s="7"/>
       <c r="BE6" s="7"/>
@@ -1661,7 +1613,9 @@
       <c r="BK6" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL6" s="12"/>
+      <c r="BL6" s="12" t="n">
+        <v>4</v>
+      </c>
       <c r="BM6" s="12"/>
       <c r="BN6" s="12"/>
       <c r="BO6" s="12"/>
@@ -1710,8 +1664,8 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="7"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="6"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
@@ -1720,8 +1674,8 @@
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="7"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="6"/>
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
       <c r="U7" s="7"/>
@@ -1745,8 +1699,8 @@
       <c r="AM7" s="7"/>
       <c r="AN7" s="7"/>
       <c r="AO7" s="6"/>
-      <c r="AP7" s="15"/>
-      <c r="AQ7" s="15"/>
+      <c r="AP7" s="7"/>
+      <c r="AQ7" s="7"/>
       <c r="AR7" s="7" t="s">
         <v>5</v>
       </c>
@@ -1771,7 +1725,9 @@
       <c r="BK7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL7" s="12"/>
+      <c r="BL7" s="12" t="n">
+        <v>5</v>
+      </c>
       <c r="BM7" s="12"/>
       <c r="BN7" s="12"/>
       <c r="BO7" s="12"/>
@@ -1820,8 +1776,8 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="6"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
@@ -1830,7 +1786,7 @@
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
-      <c r="Q8" s="6"/>
+      <c r="Q8" s="18"/>
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
@@ -1839,7 +1795,7 @@
       </c>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
+      <c r="X8" s="19"/>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
       <c r="AA8" s="6"/>
@@ -1857,8 +1813,8 @@
       <c r="AM8" s="7"/>
       <c r="AN8" s="7"/>
       <c r="AO8" s="6"/>
-      <c r="AP8" s="15"/>
-      <c r="AQ8" s="15"/>
+      <c r="AP8" s="7"/>
+      <c r="AQ8" s="7"/>
       <c r="AR8" s="7"/>
       <c r="AS8" s="7"/>
       <c r="AT8" s="6"/>
@@ -1881,7 +1837,9 @@
       <c r="BK8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL8" s="12"/>
+      <c r="BL8" s="12" t="n">
+        <v>6</v>
+      </c>
       <c r="BM8" s="12"/>
       <c r="BN8" s="12"/>
       <c r="BO8" s="12"/>
@@ -1932,8 +1890,8 @@
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
+      <c r="G9" s="18"/>
+      <c r="H9" s="6"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
@@ -1942,14 +1900,14 @@
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="8"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="6"/>
       <c r="S9" s="8"/>
       <c r="T9" s="8"/>
       <c r="U9" s="7"/>
       <c r="V9" s="8"/>
       <c r="W9" s="8"/>
-      <c r="X9" s="8"/>
+      <c r="X9" s="20"/>
       <c r="Y9" s="8"/>
       <c r="Z9" s="8"/>
       <c r="AA9" s="8"/>
@@ -1963,12 +1921,14 @@
       <c r="AI9" s="7"/>
       <c r="AJ9" s="6"/>
       <c r="AK9" s="7"/>
-      <c r="AL9" s="7"/>
+      <c r="AL9" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="AM9" s="7"/>
       <c r="AN9" s="7"/>
       <c r="AO9" s="6"/>
-      <c r="AP9" s="15"/>
-      <c r="AQ9" s="15"/>
+      <c r="AP9" s="7"/>
+      <c r="AQ9" s="7"/>
       <c r="AR9" s="7"/>
       <c r="AS9" s="7"/>
       <c r="AT9" s="6"/>
@@ -1991,7 +1951,9 @@
       <c r="BK9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL9" s="12"/>
+      <c r="BL9" s="12" t="n">
+        <v>7</v>
+      </c>
       <c r="BM9" s="12"/>
       <c r="BN9" s="12"/>
       <c r="BO9" s="12"/>
@@ -2040,8 +2002,8 @@
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="7"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="8"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
@@ -2050,8 +2012,8 @@
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="7"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="6"/>
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
       <c r="U10" s="7"/>
@@ -2075,8 +2037,8 @@
       <c r="AM10" s="7"/>
       <c r="AN10" s="7"/>
       <c r="AO10" s="6"/>
-      <c r="AP10" s="15"/>
-      <c r="AQ10" s="15"/>
+      <c r="AP10" s="7"/>
+      <c r="AQ10" s="7"/>
       <c r="AR10" s="7"/>
       <c r="AS10" s="7"/>
       <c r="AT10" s="6"/>
@@ -2099,7 +2061,9 @@
       <c r="BK10" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL10" s="12"/>
+      <c r="BL10" s="12" t="n">
+        <v>8</v>
+      </c>
       <c r="BM10" s="12"/>
       <c r="BN10" s="12"/>
       <c r="BO10" s="12"/>
@@ -2148,7 +2112,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="G11" s="18"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
@@ -2158,15 +2122,15 @@
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="7"/>
+      <c r="Q11" s="18"/>
+      <c r="R11" s="6"/>
       <c r="S11" s="7"/>
-      <c r="T11" s="6"/>
-      <c r="U11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="6"/>
       <c r="V11" s="7"/>
       <c r="W11" s="7"/>
       <c r="X11" s="7"/>
-      <c r="Y11" s="6"/>
+      <c r="Y11" s="7"/>
       <c r="Z11" s="7"/>
       <c r="AA11" s="7"/>
       <c r="AB11" s="7"/>
@@ -2183,8 +2147,8 @@
       <c r="AM11" s="7"/>
       <c r="AN11" s="7"/>
       <c r="AO11" s="6"/>
-      <c r="AP11" s="15"/>
-      <c r="AQ11" s="15"/>
+      <c r="AP11" s="7"/>
+      <c r="AQ11" s="7"/>
       <c r="AR11" s="7"/>
       <c r="AS11" s="7"/>
       <c r="AT11" s="6"/>
@@ -2207,7 +2171,9 @@
       <c r="BK11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL11" s="12"/>
+      <c r="BL11" s="12" t="n">
+        <v>9</v>
+      </c>
       <c r="BM11" s="12"/>
       <c r="BN11" s="12"/>
       <c r="BO11" s="12"/>
@@ -2256,8 +2222,8 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
+      <c r="G12" s="19"/>
+      <c r="H12" s="6"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7" t="s">
         <v>5</v>
@@ -2266,17 +2232,19 @@
       <c r="L12" s="6"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
+      <c r="O12" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="P12" s="7"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="7"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="6"/>
       <c r="S12" s="7"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="8"/>
       <c r="V12" s="7"/>
       <c r="W12" s="7"/>
       <c r="X12" s="7"/>
-      <c r="Y12" s="8"/>
+      <c r="Y12" s="7"/>
       <c r="Z12" s="7"/>
       <c r="AA12" s="7"/>
       <c r="AB12" s="7"/>
@@ -2293,8 +2261,8 @@
       <c r="AM12" s="7"/>
       <c r="AN12" s="7"/>
       <c r="AO12" s="6"/>
-      <c r="AP12" s="15"/>
-      <c r="AQ12" s="15"/>
+      <c r="AP12" s="7"/>
+      <c r="AQ12" s="7"/>
       <c r="AR12" s="7"/>
       <c r="AS12" s="7"/>
       <c r="AT12" s="6"/>
@@ -2317,7 +2285,9 @@
       <c r="BK12" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL12" s="12"/>
+      <c r="BL12" s="12" t="n">
+        <v>10</v>
+      </c>
       <c r="BM12" s="12"/>
       <c r="BN12" s="12"/>
       <c r="BO12" s="12"/>
@@ -2366,8 +2336,8 @@
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="7"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="6"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
       <c r="K13" s="7"/>
@@ -2376,8 +2346,8 @@
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="7"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="6"/>
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
       <c r="U13" s="7"/>
@@ -2401,8 +2371,8 @@
       <c r="AM13" s="7"/>
       <c r="AN13" s="7"/>
       <c r="AO13" s="6"/>
-      <c r="AP13" s="15"/>
-      <c r="AQ13" s="15"/>
+      <c r="AP13" s="7"/>
+      <c r="AQ13" s="7"/>
       <c r="AR13" s="7"/>
       <c r="AS13" s="7"/>
       <c r="AT13" s="6"/>
@@ -2427,7 +2397,9 @@
       <c r="BK13" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL13" s="12"/>
+      <c r="BL13" s="12" t="n">
+        <v>11</v>
+      </c>
       <c r="BM13" s="12"/>
       <c r="BN13" s="12"/>
       <c r="BO13" s="12"/>
@@ -2476,8 +2448,8 @@
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="6"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
@@ -2486,8 +2458,8 @@
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="7"/>
+      <c r="Q14" s="18"/>
+      <c r="R14" s="6"/>
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>
@@ -2511,8 +2483,8 @@
       <c r="AM14" s="7"/>
       <c r="AN14" s="7"/>
       <c r="AO14" s="6"/>
-      <c r="AP14" s="15"/>
-      <c r="AQ14" s="15"/>
+      <c r="AP14" s="7"/>
+      <c r="AQ14" s="7"/>
       <c r="AR14" s="7"/>
       <c r="AS14" s="7"/>
       <c r="AT14" s="6"/>
@@ -2535,7 +2507,9 @@
       <c r="BK14" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL14" s="12"/>
+      <c r="BL14" s="12" t="n">
+        <v>12</v>
+      </c>
       <c r="BM14" s="12"/>
       <c r="BN14" s="12"/>
       <c r="BO14" s="12"/>
@@ -2586,10 +2560,10 @@
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="18"/>
+      <c r="H15" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
@@ -2598,8 +2572,8 @@
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="7"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="6"/>
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
       <c r="U15" s="7"/>
@@ -2625,14 +2599,16 @@
       <c r="AM15" s="7"/>
       <c r="AN15" s="6"/>
       <c r="AO15" s="6"/>
-      <c r="AP15" s="19"/>
-      <c r="AQ15" s="19"/>
+      <c r="AP15" s="6"/>
+      <c r="AQ15" s="6"/>
       <c r="AR15" s="7"/>
       <c r="AS15" s="6"/>
       <c r="AT15" s="6"/>
       <c r="AU15" s="6"/>
       <c r="AV15" s="6"/>
-      <c r="AW15" s="7"/>
+      <c r="AW15" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="AX15" s="6"/>
       <c r="AY15" s="6"/>
       <c r="AZ15" s="7"/>
@@ -2649,7 +2625,9 @@
       <c r="BK15" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL15" s="12"/>
+      <c r="BL15" s="12" t="n">
+        <v>13</v>
+      </c>
       <c r="BM15" s="12"/>
       <c r="BN15" s="12"/>
       <c r="BO15" s="12"/>
@@ -2698,8 +2676,8 @@
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="6"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
@@ -2708,8 +2686,8 @@
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="7"/>
+      <c r="Q16" s="18"/>
+      <c r="R16" s="6"/>
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
@@ -2733,8 +2711,8 @@
       <c r="AM16" s="7"/>
       <c r="AN16" s="8"/>
       <c r="AO16" s="6"/>
-      <c r="AP16" s="16"/>
-      <c r="AQ16" s="16"/>
+      <c r="AP16" s="8"/>
+      <c r="AQ16" s="8"/>
       <c r="AR16" s="7"/>
       <c r="AS16" s="8"/>
       <c r="AT16" s="6"/>
@@ -2757,7 +2735,9 @@
       <c r="BK16" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL16" s="12"/>
+      <c r="BL16" s="12" t="n">
+        <v>14</v>
+      </c>
       <c r="BM16" s="12"/>
       <c r="BN16" s="12"/>
       <c r="BO16" s="12"/>
@@ -2806,18 +2786,18 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="7"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="7"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="18"/>
+      <c r="Q17" s="18"/>
+      <c r="R17" s="6"/>
       <c r="S17" s="7"/>
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
@@ -2843,8 +2823,8 @@
       <c r="AM17" s="7"/>
       <c r="AN17" s="7"/>
       <c r="AO17" s="6"/>
-      <c r="AP17" s="15"/>
-      <c r="AQ17" s="15"/>
+      <c r="AP17" s="7"/>
+      <c r="AQ17" s="7"/>
       <c r="AR17" s="7"/>
       <c r="AS17" s="7"/>
       <c r="AT17" s="6"/>
@@ -2869,7 +2849,9 @@
       <c r="BK17" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL17" s="12"/>
+      <c r="BL17" s="12" t="n">
+        <v>15</v>
+      </c>
       <c r="BM17" s="12"/>
       <c r="BN17" s="12"/>
       <c r="BO17" s="12"/>
@@ -2918,25 +2900,25 @@
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="7"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="6"/>
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="7"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="18"/>
+      <c r="Q18" s="18"/>
+      <c r="R18" s="6"/>
       <c r="S18" s="7"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="6"/>
       <c r="V18" s="7"/>
       <c r="W18" s="7"/>
       <c r="X18" s="7"/>
-      <c r="Y18" s="6"/>
+      <c r="Y18" s="7"/>
       <c r="Z18" s="7"/>
       <c r="AA18" s="7"/>
       <c r="AB18" s="7"/>
@@ -2953,10 +2935,10 @@
       <c r="AM18" s="7"/>
       <c r="AN18" s="7"/>
       <c r="AO18" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="AP18" s="15"/>
-      <c r="AQ18" s="15"/>
+        <v>8</v>
+      </c>
+      <c r="AP18" s="7"/>
+      <c r="AQ18" s="7"/>
       <c r="AR18" s="7"/>
       <c r="AS18" s="7"/>
       <c r="AT18" s="6"/>
@@ -2967,7 +2949,7 @@
       <c r="AY18" s="6"/>
       <c r="AZ18" s="6"/>
       <c r="BA18" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="BB18" s="6"/>
       <c r="BC18" s="6"/>
@@ -2981,7 +2963,9 @@
       <c r="BK18" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL18" s="12"/>
+      <c r="BL18" s="12" t="n">
+        <v>16</v>
+      </c>
       <c r="BM18" s="12"/>
       <c r="BN18" s="12"/>
       <c r="BO18" s="12"/>
@@ -3028,12 +3012,12 @@
       <c r="B19" s="5"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="7"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="8"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
@@ -3044,15 +3028,15 @@
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="7"/>
+      <c r="Q19" s="18"/>
+      <c r="R19" s="6"/>
       <c r="S19" s="7"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="8"/>
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
-      <c r="Y19" s="8"/>
+      <c r="Y19" s="7"/>
       <c r="Z19" s="7"/>
       <c r="AA19" s="7"/>
       <c r="AB19" s="7"/>
@@ -3069,8 +3053,8 @@
       <c r="AM19" s="7"/>
       <c r="AN19" s="7"/>
       <c r="AO19" s="6"/>
-      <c r="AP19" s="15"/>
-      <c r="AQ19" s="15"/>
+      <c r="AP19" s="7"/>
+      <c r="AQ19" s="7"/>
       <c r="AR19" s="7"/>
       <c r="AS19" s="7"/>
       <c r="AT19" s="6"/>
@@ -3093,7 +3077,9 @@
       <c r="BK19" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL19" s="12"/>
+      <c r="BL19" s="12" t="n">
+        <v>17</v>
+      </c>
       <c r="BM19" s="12"/>
       <c r="BN19" s="12"/>
       <c r="BO19" s="12"/>
@@ -3152,11 +3138,11 @@
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="7" t="s">
+      <c r="Q20" s="18"/>
+      <c r="R20" s="6"/>
+      <c r="S20" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="S20" s="7"/>
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
       <c r="V20" s="7"/>
@@ -3179,8 +3165,8 @@
       <c r="AM20" s="7"/>
       <c r="AN20" s="7"/>
       <c r="AO20" s="6"/>
-      <c r="AP20" s="15"/>
-      <c r="AQ20" s="15"/>
+      <c r="AP20" s="7"/>
+      <c r="AQ20" s="7"/>
       <c r="AR20" s="7"/>
       <c r="AS20" s="7"/>
       <c r="AT20" s="6"/>
@@ -3205,7 +3191,9 @@
       <c r="BK20" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="BL20" s="12"/>
+      <c r="BL20" s="12" t="n">
+        <v>18</v>
+      </c>
       <c r="BM20" s="12"/>
       <c r="BN20" s="12"/>
       <c r="BO20" s="12"/>
@@ -3289,8 +3277,8 @@
       <c r="AM21" s="5"/>
       <c r="AN21" s="5"/>
       <c r="AO21" s="5"/>
-      <c r="AP21" s="14"/>
-      <c r="AQ21" s="14"/>
+      <c r="AP21" s="10"/>
+      <c r="AQ21" s="10"/>
       <c r="AR21" s="10"/>
       <c r="AS21" s="10"/>
       <c r="AT21" s="10"/>
@@ -3313,7 +3301,9 @@
       <c r="BK21" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="BL21" s="12"/>
+      <c r="BL21" s="12" t="n">
+        <v>19</v>
+      </c>
       <c r="BM21" s="12"/>
       <c r="BN21" s="12"/>
       <c r="BO21" s="12"/>
@@ -3358,7 +3348,7 @@
         <v>5</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
@@ -3372,7 +3362,7 @@
         <v>3</v>
       </c>
       <c r="M22" s="13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N22" s="13"/>
       <c r="O22" s="13"/>
@@ -3383,10 +3373,10 @@
     </row>
     <row r="23" spans="2:19">
       <c r="B23" s="13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
@@ -3400,7 +3390,7 @@
         <v>7</v>
       </c>
       <c r="M23" s="13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="N23" s="13"/>
       <c r="O23" s="13"/>
@@ -3410,9 +3400,9 @@
       <c r="S23" s="13"/>
     </row>
     <row r="24" spans="2:19">
-      <c r="B24" s="20"/>
+      <c r="B24" s="15"/>
       <c r="C24" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
@@ -3426,7 +3416,7 @@
         <v>1</v>
       </c>
       <c r="M24" s="13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N24" s="13"/>
       <c r="O24" s="13"/>
@@ -3436,15 +3426,15 @@
       <c r="S24" s="13"/>
     </row>
     <row r="25" spans="2:19">
-      <c r="B25" s="21"/>
-      <c r="C25" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
       <c r="K25" s="13"/>
@@ -3452,7 +3442,7 @@
         <v>2</v>
       </c>
       <c r="M25" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N25" s="13"/>
       <c r="O25" s="13"/>
@@ -3462,9 +3452,9 @@
       <c r="S25" s="13"/>
     </row>
     <row r="26" spans="2:19">
-      <c r="B26" s="22"/>
+      <c r="B26" s="17"/>
       <c r="C26" s="13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
@@ -3475,10 +3465,10 @@
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M26" s="13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N26" s="13"/>
       <c r="O26" s="13"/>
@@ -3489,10 +3479,10 @@
     </row>
     <row r="27" spans="2:19">
       <c r="B27" s="13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
@@ -3506,7 +3496,7 @@
         <v>6</v>
       </c>
       <c r="M27" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
@@ -3517,10 +3507,10 @@
     </row>
     <row r="28" spans="2:19">
       <c r="B28" s="13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
@@ -3541,10 +3531,10 @@
     </row>
     <row r="29" spans="2:19">
       <c r="B29" s="13" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
@@ -3564,13 +3554,13 @@
       <c r="S29" s="13"/>
     </row>
     <row r="30" spans="2:19">
-      <c r="B30" s="17"/>
-      <c r="C30" s="17"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
       <c r="I30" s="13"/>
       <c r="J30" s="13"/>
       <c r="K30" s="13"/>
@@ -3692,7 +3682,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1585955463" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1585986283" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -3701,16 +3691,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1585955463" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1585955463" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1585955463" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1585955463" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1585986283" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1585986283" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1585986283" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1585986283" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1585955463" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1585986283" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Needs the map Exit function and Combat
</commit_message>
<xml_diff>
--- a/template mapas.xlsx
+++ b/template mapas.xlsx
@@ -13,17 +13,17 @@
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1585986283" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1585986283" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1585986283" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1585986283"/>
+      <pm:revision xmlns:pm="smNativeData" day="1586161829" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1586161829" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1586161829" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1586161829"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="54">
   <si>
     <t>x</t>
   </si>
@@ -46,15 +46,12 @@
     <t>L</t>
   </si>
   <si>
+    <t>P</t>
+  </si>
+  <si>
     <t>\</t>
   </si>
   <si>
-    <t>|</t>
-  </si>
-  <si>
-    <t>_</t>
-  </si>
-  <si>
     <t>p</t>
   </si>
   <si>
@@ -64,30 +61,78 @@
     <t>DOOR</t>
   </si>
   <si>
+    <t>map01[13][6] = V_DOOR;</t>
+  </si>
+  <si>
+    <t>map01[14][11] = KEY;</t>
+  </si>
+  <si>
+    <t>map01[3][16] = BARRIER;</t>
+  </si>
+  <si>
+    <t>map01[8][2] = LORE;</t>
+  </si>
+  <si>
     <t>PLAYER</t>
   </si>
   <si>
     <t>LEVER</t>
   </si>
   <si>
+    <t>map01[3][6] = V_DOOR;</t>
+  </si>
+  <si>
+    <t>map01[18][30] = KEY;</t>
+  </si>
+  <si>
+    <t>map01[13][42] = BARRIER;</t>
+  </si>
+  <si>
     <t>WALL</t>
   </si>
   <si>
     <t>KEY</t>
   </si>
   <si>
+    <t>map01[6][19] = H_DOOR;</t>
+  </si>
+  <si>
+    <t>map01[12][35] = KEY;</t>
+  </si>
+  <si>
+    <t>map01[5][59] = BARRIER;</t>
+  </si>
+  <si>
     <t>INNER WALL</t>
   </si>
   <si>
     <t>WEAPON</t>
   </si>
   <si>
+    <t>map01[6][33] = H_DOOR;</t>
+  </si>
+  <si>
+    <t>map01[2][40] = KEY;</t>
+  </si>
+  <si>
+    <t>map01[10][14] = ENEMY;</t>
+  </si>
+  <si>
     <t>FLOOR</t>
   </si>
   <si>
     <t>BARRIER</t>
   </si>
   <si>
+    <t>map01[16][39] = V_DOOR;</t>
+  </si>
+  <si>
+    <t>map01[18][45] = KEY;</t>
+  </si>
+  <si>
+    <t>map01[13][21] = ENEMY;</t>
+  </si>
+  <si>
     <t>X</t>
   </si>
   <si>
@@ -97,13 +142,49 @@
     <t>LORE</t>
   </si>
   <si>
+    <t>map01[13][47] = H_DOOR;</t>
+  </si>
+  <si>
+    <t>map01[7][50] = KEY;</t>
+  </si>
+  <si>
+    <t>map01[12][28] = ENEMY;</t>
+  </si>
+  <si>
     <t>POTION</t>
   </si>
   <si>
+    <t>map01[16][51] = H_DOOR;</t>
+  </si>
+  <si>
+    <t>map01[16][11] = LEVER_ON;</t>
+  </si>
+  <si>
+    <t>map01[17][34] = ENEMY;</t>
+  </si>
+  <si>
     <t>q</t>
   </si>
   <si>
     <t>QUEST ITEM</t>
+  </si>
+  <si>
+    <t>map01[3][2] = WEAPON;</t>
+  </si>
+  <si>
+    <t>map01[14][32] = LEVER_ON;</t>
+  </si>
+  <si>
+    <t>map01[7][47] = ENEMY;</t>
+  </si>
+  <si>
+    <t>map01[13][2] = POTION;</t>
+  </si>
+  <si>
+    <t>map01[17][59] = LEVER_ON;</t>
+  </si>
+  <si>
+    <t>map01[11][54] = ENEMY;</t>
   </si>
 </sst>
 </file>
@@ -120,7 +201,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;R$&quot;_-;\-* #,##0.00\ &quot;R$&quot;_-;_-* &quot;-&quot;??\ &quot;R$&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _R_$_-;\-* #,##0.00\ _R_$_-;_-* &quot;-&quot;??\ _R_$_-;_-@_-"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -128,7 +209,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1585986283" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1586161829" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -144,7 +225,7 @@
       <sz val="20"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1585986283" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1586161829" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="400" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -160,8 +241,24 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1585986283" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1586161829" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
+            <pm:cs face="Times New Roman" sz="200" lang="default"/>
+            <pm:ea face="SimSun" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <b/>
+      <color rgb="FF000000"/>
+      <sz val="16"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1586161829" ulstyle="none" kern="1">
+            <pm:latin face="Arial" sz="320" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
           </pm:charSpec>
@@ -182,7 +279,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -193,7 +290,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="71" fgClr="00FFFFFF" bgLvl="29" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="71" fgClr="00FFFFFF" bgLvl="29" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -204,7 +301,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="0" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="0" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -215,7 +312,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="100" fgClr="004D4D4D" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="100" fgClr="004D4D4D" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -226,7 +323,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="100" fgClr="00B3B3B3" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="100" fgClr="00B3B3B3" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -237,7 +334,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="100" fgClr="007F7F7F" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="100" fgClr="007F7F7F" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -248,7 +345,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="100" fgClr="00000000" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="100" fgClr="00000000" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -259,7 +356,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -270,7 +367,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -281,7 +378,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1585986283" type="1" fgLvl="100" fgClr="00333333" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="100" fgClr="00333333" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -303,7 +400,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
+          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
         </ext>
       </extLst>
     </border>
@@ -322,7 +419,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
+          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
         </ext>
       </extLst>
     </border>
@@ -341,7 +438,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
+          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
         </ext>
       </extLst>
     </border>
@@ -360,7 +457,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
+          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
         </ext>
       </extLst>
     </border>
@@ -379,7 +476,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
+          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
         </ext>
       </extLst>
     </border>
@@ -398,7 +495,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
+          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
         </ext>
       </extLst>
     </border>
@@ -417,7 +514,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
+          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
         </ext>
       </extLst>
     </border>
@@ -436,7 +533,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
+          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
         </ext>
       </extLst>
     </border>
@@ -455,7 +552,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
+          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
         </ext>
       </extLst>
     </border>
@@ -474,7 +571,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
+          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
         </ext>
       </extLst>
     </border>
@@ -493,7 +590,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1585986283"/>
+          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
         </ext>
       </extLst>
     </border>
@@ -501,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -554,17 +651,8 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -573,10 +661,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1585986283" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1586161829" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1585986283" count="4">
+      <pm:colors xmlns:pm="smNativeData" id="1586161829" count="4">
         <pm:color name="Cor 24" rgb="FFFF9E"/>
         <pm:color name="Cor 25" rgb="B5B5B5"/>
         <pm:color name="Cor 26" rgb="6B6B6B"/>
@@ -845,8 +933,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CZ65"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" topLeftCell="AC1" zoomScale="60" workbookViewId="0">
-      <selection activeCell="AU18" sqref="AU18"/>
+    <sheetView tabSelected="1" view="normal" zoomScale="60" workbookViewId="0">
+      <selection activeCell="X22" sqref="X22:AI22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="24.95"/>
@@ -1110,7 +1198,7 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="21"/>
+      <c r="Q2" s="10"/>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
@@ -1210,7 +1298,7 @@
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
-      <c r="G3" s="20"/>
+      <c r="G3" s="8"/>
       <c r="H3" s="6"/>
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
@@ -1220,7 +1308,7 @@
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
       <c r="P3" s="8"/>
-      <c r="Q3" s="20"/>
+      <c r="Q3" s="8"/>
       <c r="R3" s="6"/>
       <c r="S3" s="8"/>
       <c r="T3" s="8"/>
@@ -1320,7 +1408,7 @@
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
-      <c r="G4" s="18"/>
+      <c r="G4" s="7"/>
       <c r="H4" s="6"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
@@ -1330,7 +1418,7 @@
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
-      <c r="Q4" s="18"/>
+      <c r="Q4" s="7"/>
       <c r="R4" s="8"/>
       <c r="S4" s="7"/>
       <c r="T4" s="7"/>
@@ -1353,11 +1441,11 @@
       <c r="AK4" s="7"/>
       <c r="AL4" s="7"/>
       <c r="AM4" s="7"/>
-      <c r="AN4" s="7" t="s">
+      <c r="AN4" s="7"/>
+      <c r="AO4" s="6"/>
+      <c r="AP4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="AO4" s="6"/>
-      <c r="AP4" s="7"/>
       <c r="AQ4" s="7"/>
       <c r="AR4" s="7"/>
       <c r="AS4" s="7"/>
@@ -1438,7 +1526,7 @@
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="18"/>
+      <c r="G5" s="7"/>
       <c r="H5" s="7" t="s">
         <v>3</v>
       </c>
@@ -1450,7 +1538,7 @@
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
-      <c r="Q5" s="18"/>
+      <c r="Q5" s="7"/>
       <c r="R5" s="7" t="s">
         <v>4</v>
       </c>
@@ -1552,7 +1640,7 @@
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
-      <c r="G6" s="18"/>
+      <c r="G6" s="7"/>
       <c r="H6" s="6"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
@@ -1562,7 +1650,7 @@
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
-      <c r="Q6" s="18"/>
+      <c r="Q6" s="7"/>
       <c r="R6" s="6"/>
       <c r="S6" s="7"/>
       <c r="T6" s="7"/>
@@ -1599,9 +1687,7 @@
       <c r="AY6" s="6"/>
       <c r="AZ6" s="7"/>
       <c r="BA6" s="7"/>
-      <c r="BB6" s="7" t="s">
-        <v>4</v>
-      </c>
+      <c r="BB6" s="7"/>
       <c r="BC6" s="7"/>
       <c r="BD6" s="7"/>
       <c r="BE6" s="7"/>
@@ -1664,7 +1750,7 @@
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
-      <c r="G7" s="19"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
@@ -1674,7 +1760,7 @@
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
-      <c r="Q7" s="18"/>
+      <c r="Q7" s="7"/>
       <c r="R7" s="6"/>
       <c r="S7" s="7"/>
       <c r="T7" s="7"/>
@@ -1701,9 +1787,7 @@
       <c r="AO7" s="6"/>
       <c r="AP7" s="7"/>
       <c r="AQ7" s="7"/>
-      <c r="AR7" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="AR7" s="7"/>
       <c r="AS7" s="7"/>
       <c r="AT7" s="6"/>
       <c r="AU7" s="7"/>
@@ -1720,7 +1804,9 @@
       <c r="BF7" s="6"/>
       <c r="BG7" s="6"/>
       <c r="BH7" s="6"/>
-      <c r="BI7" s="7"/>
+      <c r="BI7" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="BJ7" s="5"/>
       <c r="BK7" s="4" t="s">
         <v>0</v>
@@ -1776,7 +1862,7 @@
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="20"/>
+      <c r="G8" s="8"/>
       <c r="H8" s="6"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
@@ -1786,7 +1872,7 @@
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
-      <c r="Q8" s="18"/>
+      <c r="Q8" s="7"/>
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
@@ -1795,7 +1881,7 @@
       </c>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
-      <c r="X8" s="19"/>
+      <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
       <c r="AA8" s="6"/>
@@ -1806,7 +1892,9 @@
       <c r="AF8" s="6"/>
       <c r="AG8" s="6"/>
       <c r="AH8" s="6"/>
-      <c r="AI8" s="7"/>
+      <c r="AI8" s="7" t="s">
+        <v>3</v>
+      </c>
       <c r="AJ8" s="6"/>
       <c r="AK8" s="7"/>
       <c r="AL8" s="7"/>
@@ -1884,13 +1972,11 @@
         <v>7</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="18"/>
+      <c r="G9" s="7"/>
       <c r="H9" s="6"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
@@ -1900,14 +1986,14 @@
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
-      <c r="Q9" s="18"/>
+      <c r="Q9" s="7"/>
       <c r="R9" s="6"/>
       <c r="S9" s="8"/>
       <c r="T9" s="8"/>
       <c r="U9" s="7"/>
       <c r="V9" s="8"/>
       <c r="W9" s="8"/>
-      <c r="X9" s="20"/>
+      <c r="X9" s="8"/>
       <c r="Y9" s="8"/>
       <c r="Z9" s="8"/>
       <c r="AA9" s="8"/>
@@ -1921,9 +2007,7 @@
       <c r="AI9" s="7"/>
       <c r="AJ9" s="6"/>
       <c r="AK9" s="7"/>
-      <c r="AL9" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="AL9" s="7"/>
       <c r="AM9" s="7"/>
       <c r="AN9" s="7"/>
       <c r="AO9" s="6"/>
@@ -1934,10 +2018,14 @@
       <c r="AT9" s="6"/>
       <c r="AU9" s="7"/>
       <c r="AV9" s="7"/>
-      <c r="AW9" s="7"/>
+      <c r="AW9" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="AX9" s="7"/>
       <c r="AY9" s="6"/>
-      <c r="AZ9" s="7"/>
+      <c r="AZ9" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="BA9" s="7"/>
       <c r="BB9" s="7"/>
       <c r="BC9" s="7"/>
@@ -1999,10 +2087,12 @@
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
-      <c r="G10" s="18"/>
+      <c r="G10" s="7"/>
       <c r="H10" s="8"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
@@ -2012,7 +2102,7 @@
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
-      <c r="Q10" s="18"/>
+      <c r="Q10" s="7"/>
       <c r="R10" s="6"/>
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
@@ -2112,7 +2202,7 @@
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
-      <c r="G11" s="18"/>
+      <c r="G11" s="7"/>
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
@@ -2122,7 +2212,7 @@
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
-      <c r="Q11" s="18"/>
+      <c r="Q11" s="7"/>
       <c r="R11" s="6"/>
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
@@ -2222,21 +2312,19 @@
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="19"/>
+      <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="J12" s="7"/>
       <c r="K12" s="7"/>
       <c r="L12" s="6"/>
       <c r="M12" s="7"/>
       <c r="N12" s="7"/>
-      <c r="O12" s="7" t="s">
+      <c r="O12" s="7"/>
+      <c r="P12" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="18"/>
+      <c r="Q12" s="7"/>
       <c r="R12" s="6"/>
       <c r="S12" s="7"/>
       <c r="T12" s="7"/>
@@ -2336,7 +2424,7 @@
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
-      <c r="G13" s="20"/>
+      <c r="G13" s="8"/>
       <c r="H13" s="6"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
@@ -2346,7 +2434,7 @@
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
-      <c r="Q13" s="18"/>
+      <c r="Q13" s="7"/>
       <c r="R13" s="6"/>
       <c r="S13" s="7"/>
       <c r="T13" s="7"/>
@@ -2385,10 +2473,10 @@
       <c r="BA13" s="7"/>
       <c r="BB13" s="7"/>
       <c r="BC13" s="7"/>
-      <c r="BD13" s="7"/>
-      <c r="BE13" s="7" t="s">
+      <c r="BD13" s="7" t="s">
         <v>5</v>
       </c>
+      <c r="BE13" s="7"/>
       <c r="BF13" s="7"/>
       <c r="BG13" s="7"/>
       <c r="BH13" s="7"/>
@@ -2448,7 +2536,7 @@
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
-      <c r="G14" s="18"/>
+      <c r="G14" s="7"/>
       <c r="H14" s="6"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
@@ -2458,7 +2546,7 @@
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
-      <c r="Q14" s="18"/>
+      <c r="Q14" s="7"/>
       <c r="R14" s="6"/>
       <c r="S14" s="7"/>
       <c r="T14" s="7"/>
@@ -2471,14 +2559,18 @@
       <c r="AA14" s="7"/>
       <c r="AB14" s="7"/>
       <c r="AC14" s="7"/>
-      <c r="AD14" s="7"/>
+      <c r="AD14" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="AE14" s="7"/>
       <c r="AF14" s="7"/>
       <c r="AG14" s="6"/>
       <c r="AH14" s="7"/>
       <c r="AI14" s="7"/>
       <c r="AJ14" s="6"/>
-      <c r="AK14" s="7"/>
+      <c r="AK14" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="AL14" s="7"/>
       <c r="AM14" s="7"/>
       <c r="AN14" s="7"/>
@@ -2554,13 +2646,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="G15" s="18"/>
+      <c r="G15" s="7"/>
       <c r="H15" s="7" t="s">
         <v>3</v>
       </c>
@@ -2572,17 +2664,17 @@
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
-      <c r="Q15" s="18"/>
+      <c r="Q15" s="7"/>
       <c r="R15" s="6"/>
       <c r="S15" s="7"/>
       <c r="T15" s="7"/>
       <c r="U15" s="7"/>
       <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
+      <c r="W15" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="X15" s="7"/>
-      <c r="Y15" s="7" t="s">
-        <v>5</v>
-      </c>
+      <c r="Y15" s="7"/>
       <c r="Z15" s="7"/>
       <c r="AA15" s="7"/>
       <c r="AB15" s="7"/>
@@ -2601,13 +2693,15 @@
       <c r="AO15" s="6"/>
       <c r="AP15" s="6"/>
       <c r="AQ15" s="6"/>
-      <c r="AR15" s="7"/>
+      <c r="AR15" s="7" t="s">
+        <v>4</v>
+      </c>
       <c r="AS15" s="6"/>
       <c r="AT15" s="6"/>
       <c r="AU15" s="6"/>
       <c r="AV15" s="6"/>
       <c r="AW15" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AX15" s="6"/>
       <c r="AY15" s="6"/>
@@ -2676,17 +2770,19 @@
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
-      <c r="G16" s="18"/>
+      <c r="G16" s="7"/>
       <c r="H16" s="6"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="6"/>
-      <c r="M16" s="7"/>
+      <c r="M16" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
-      <c r="Q16" s="18"/>
+      <c r="Q16" s="7"/>
       <c r="R16" s="6"/>
       <c r="S16" s="7"/>
       <c r="T16" s="7"/>
@@ -2703,7 +2799,9 @@
       <c r="AE16" s="7"/>
       <c r="AF16" s="7"/>
       <c r="AG16" s="6"/>
-      <c r="AH16" s="8"/>
+      <c r="AH16" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="AI16" s="8"/>
       <c r="AJ16" s="8"/>
       <c r="AK16" s="8"/>
@@ -2786,7 +2884,7 @@
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
-      <c r="G17" s="19"/>
+      <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -2795,8 +2893,8 @@
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
       <c r="R17" s="6"/>
       <c r="S17" s="7"/>
       <c r="T17" s="7"/>
@@ -2813,9 +2911,7 @@
       <c r="AE17" s="7"/>
       <c r="AF17" s="7"/>
       <c r="AG17" s="6"/>
-      <c r="AH17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="AH17" s="7"/>
       <c r="AI17" s="7"/>
       <c r="AJ17" s="7"/>
       <c r="AK17" s="7"/>
@@ -2828,9 +2924,7 @@
       <c r="AR17" s="7"/>
       <c r="AS17" s="7"/>
       <c r="AT17" s="6"/>
-      <c r="AU17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="AU17" s="7"/>
       <c r="AV17" s="7"/>
       <c r="AW17" s="7"/>
       <c r="AX17" s="7"/>
@@ -2900,17 +2994,19 @@
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
-      <c r="G18" s="20"/>
+      <c r="G18" s="8"/>
       <c r="H18" s="6"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="6"/>
-      <c r="M18" s="8"/>
+      <c r="M18" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
       <c r="R18" s="6"/>
       <c r="S18" s="7"/>
       <c r="T18" s="7"/>
@@ -2935,7 +3031,7 @@
       <c r="AM18" s="7"/>
       <c r="AN18" s="7"/>
       <c r="AO18" s="7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AP18" s="7"/>
       <c r="AQ18" s="7"/>
@@ -2949,7 +3045,7 @@
       <c r="AY18" s="6"/>
       <c r="AZ18" s="6"/>
       <c r="BA18" s="7" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="BB18" s="6"/>
       <c r="BC18" s="6"/>
@@ -3012,23 +3108,21 @@
       <c r="B19" s="5"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
-      <c r="G19" s="18"/>
+      <c r="G19" s="7"/>
       <c r="H19" s="8"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
       <c r="L19" s="6"/>
-      <c r="M19" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="M19" s="7"/>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
-      <c r="Q19" s="18"/>
+      <c r="Q19" s="7"/>
       <c r="R19" s="6"/>
       <c r="S19" s="7"/>
       <c r="T19" s="7"/>
@@ -3047,7 +3141,9 @@
       <c r="AG19" s="6"/>
       <c r="AH19" s="7"/>
       <c r="AI19" s="7"/>
-      <c r="AJ19" s="7"/>
+      <c r="AJ19" s="7" t="s">
+        <v>5</v>
+      </c>
       <c r="AK19" s="7"/>
       <c r="AL19" s="7"/>
       <c r="AM19" s="7"/>
@@ -3072,7 +3168,9 @@
       <c r="BF19" s="8"/>
       <c r="BG19" s="8"/>
       <c r="BH19" s="8"/>
-      <c r="BI19" s="8"/>
+      <c r="BI19" s="8" t="s">
+        <v>8</v>
+      </c>
       <c r="BJ19" s="5"/>
       <c r="BK19" s="4" t="s">
         <v>0</v>
@@ -3138,11 +3236,9 @@
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
-      <c r="Q20" s="18"/>
+      <c r="Q20" s="7"/>
       <c r="R20" s="6"/>
-      <c r="S20" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="S20" s="7"/>
       <c r="T20" s="7"/>
       <c r="U20" s="7"/>
       <c r="V20" s="7"/>
@@ -3155,7 +3251,9 @@
       <c r="AC20" s="7"/>
       <c r="AD20" s="7"/>
       <c r="AE20" s="7"/>
-      <c r="AF20" s="7"/>
+      <c r="AF20" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="AG20" s="6"/>
       <c r="AH20" s="7"/>
       <c r="AI20" s="7"/>
@@ -3170,7 +3268,9 @@
       <c r="AR20" s="7"/>
       <c r="AS20" s="7"/>
       <c r="AT20" s="6"/>
-      <c r="AU20" s="7"/>
+      <c r="AU20" s="7" t="s">
+        <v>1</v>
+      </c>
       <c r="AV20" s="7"/>
       <c r="AW20" s="7"/>
       <c r="AX20" s="7"/>
@@ -3184,9 +3284,7 @@
       <c r="BF20" s="7"/>
       <c r="BG20" s="7"/>
       <c r="BH20" s="7"/>
-      <c r="BI20" s="7" t="s">
-        <v>1</v>
-      </c>
+      <c r="BI20" s="7"/>
       <c r="BJ20" s="5"/>
       <c r="BK20" s="7" t="s">
         <v>0</v>
@@ -3343,12 +3441,12 @@
       <c r="CW21" s="12"/>
       <c r="CX21" s="12"/>
     </row>
-    <row r="22" spans="2:19">
+    <row r="22" spans="2:71">
       <c r="B22" s="13" t="s">
         <v>5</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
@@ -3362,7 +3460,7 @@
         <v>3</v>
       </c>
       <c r="M22" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N22" s="13"/>
       <c r="O22" s="13"/>
@@ -3370,13 +3468,69 @@
       <c r="Q22" s="13"/>
       <c r="R22" s="13"/>
       <c r="S22" s="13"/>
-    </row>
-    <row r="23" spans="2:19">
+      <c r="X22" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y22" s="18"/>
+      <c r="Z22" s="18"/>
+      <c r="AA22" s="18"/>
+      <c r="AB22" s="18"/>
+      <c r="AC22" s="18"/>
+      <c r="AD22" s="18"/>
+      <c r="AE22" s="18"/>
+      <c r="AF22" s="18"/>
+      <c r="AG22" s="18"/>
+      <c r="AH22" s="18"/>
+      <c r="AI22" s="18"/>
+      <c r="AJ22" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="AK22" s="18"/>
+      <c r="AL22" s="18"/>
+      <c r="AM22" s="18"/>
+      <c r="AN22" s="18"/>
+      <c r="AO22" s="18"/>
+      <c r="AP22" s="18"/>
+      <c r="AQ22" s="18"/>
+      <c r="AR22" s="18"/>
+      <c r="AS22" s="18"/>
+      <c r="AT22" s="18"/>
+      <c r="AU22" s="18"/>
+      <c r="AV22" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="AW22" s="18"/>
+      <c r="AX22" s="18"/>
+      <c r="AY22" s="18"/>
+      <c r="AZ22" s="18"/>
+      <c r="BA22" s="18"/>
+      <c r="BB22" s="18"/>
+      <c r="BC22" s="18"/>
+      <c r="BD22" s="18"/>
+      <c r="BE22" s="18"/>
+      <c r="BF22" s="18"/>
+      <c r="BG22" s="18"/>
+      <c r="BH22" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="BI22" s="18"/>
+      <c r="BJ22" s="18"/>
+      <c r="BK22" s="18"/>
+      <c r="BL22" s="18"/>
+      <c r="BM22" s="18"/>
+      <c r="BN22" s="18"/>
+      <c r="BO22" s="18"/>
+      <c r="BP22" s="18"/>
+      <c r="BQ22" s="18"/>
+      <c r="BR22" s="18"/>
+      <c r="BS22" s="18"/>
+    </row>
+    <row r="23" spans="2:71">
       <c r="B23" s="13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
@@ -3387,10 +3541,10 @@
       <c r="J23" s="13"/>
       <c r="K23" s="13"/>
       <c r="L23" s="13" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="M23" s="13" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="N23" s="13"/>
       <c r="O23" s="13"/>
@@ -3398,11 +3552,65 @@
       <c r="Q23" s="13"/>
       <c r="R23" s="13"/>
       <c r="S23" s="13"/>
-    </row>
-    <row r="24" spans="2:19">
+      <c r="X23" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y23" s="18"/>
+      <c r="Z23" s="18"/>
+      <c r="AA23" s="18"/>
+      <c r="AB23" s="18"/>
+      <c r="AC23" s="18"/>
+      <c r="AD23" s="18"/>
+      <c r="AE23" s="18"/>
+      <c r="AF23" s="18"/>
+      <c r="AG23" s="18"/>
+      <c r="AH23" s="18"/>
+      <c r="AI23" s="18"/>
+      <c r="AJ23" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK23" s="18"/>
+      <c r="AL23" s="18"/>
+      <c r="AM23" s="18"/>
+      <c r="AN23" s="18"/>
+      <c r="AO23" s="18"/>
+      <c r="AP23" s="18"/>
+      <c r="AQ23" s="18"/>
+      <c r="AR23" s="18"/>
+      <c r="AS23" s="18"/>
+      <c r="AT23" s="18"/>
+      <c r="AU23" s="18"/>
+      <c r="AV23" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="AW23" s="18"/>
+      <c r="AX23" s="18"/>
+      <c r="AY23" s="18"/>
+      <c r="AZ23" s="18"/>
+      <c r="BA23" s="18"/>
+      <c r="BB23" s="18"/>
+      <c r="BC23" s="18"/>
+      <c r="BD23" s="18"/>
+      <c r="BE23" s="18"/>
+      <c r="BF23" s="18"/>
+      <c r="BG23" s="18"/>
+      <c r="BH23" s="18"/>
+      <c r="BI23" s="18"/>
+      <c r="BJ23" s="18"/>
+      <c r="BK23" s="18"/>
+      <c r="BL23" s="18"/>
+      <c r="BM23" s="18"/>
+      <c r="BN23" s="18"/>
+      <c r="BO23" s="18"/>
+      <c r="BP23" s="18"/>
+      <c r="BQ23" s="18"/>
+      <c r="BR23" s="18"/>
+      <c r="BS23" s="18"/>
+    </row>
+    <row r="24" spans="2:71">
       <c r="B24" s="15"/>
       <c r="C24" s="13" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
@@ -3416,7 +3624,7 @@
         <v>1</v>
       </c>
       <c r="M24" s="13" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="N24" s="13"/>
       <c r="O24" s="13"/>
@@ -3424,11 +3632,65 @@
       <c r="Q24" s="13"/>
       <c r="R24" s="13"/>
       <c r="S24" s="13"/>
-    </row>
-    <row r="25" spans="2:19">
+      <c r="X24" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y24" s="18"/>
+      <c r="Z24" s="18"/>
+      <c r="AA24" s="18"/>
+      <c r="AB24" s="18"/>
+      <c r="AC24" s="18"/>
+      <c r="AD24" s="18"/>
+      <c r="AE24" s="18"/>
+      <c r="AF24" s="18"/>
+      <c r="AG24" s="18"/>
+      <c r="AH24" s="18"/>
+      <c r="AI24" s="18"/>
+      <c r="AJ24" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK24" s="18"/>
+      <c r="AL24" s="18"/>
+      <c r="AM24" s="18"/>
+      <c r="AN24" s="18"/>
+      <c r="AO24" s="18"/>
+      <c r="AP24" s="18"/>
+      <c r="AQ24" s="18"/>
+      <c r="AR24" s="18"/>
+      <c r="AS24" s="18"/>
+      <c r="AT24" s="18"/>
+      <c r="AU24" s="18"/>
+      <c r="AV24" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="AW24" s="18"/>
+      <c r="AX24" s="18"/>
+      <c r="AY24" s="18"/>
+      <c r="AZ24" s="18"/>
+      <c r="BA24" s="18"/>
+      <c r="BB24" s="18"/>
+      <c r="BC24" s="18"/>
+      <c r="BD24" s="18"/>
+      <c r="BE24" s="18"/>
+      <c r="BF24" s="18"/>
+      <c r="BG24" s="18"/>
+      <c r="BH24" s="18"/>
+      <c r="BI24" s="18"/>
+      <c r="BJ24" s="18"/>
+      <c r="BK24" s="18"/>
+      <c r="BL24" s="18"/>
+      <c r="BM24" s="18"/>
+      <c r="BN24" s="18"/>
+      <c r="BO24" s="18"/>
+      <c r="BP24" s="18"/>
+      <c r="BQ24" s="18"/>
+      <c r="BR24" s="18"/>
+      <c r="BS24" s="18"/>
+    </row>
+    <row r="25" spans="2:71">
       <c r="B25" s="16"/>
       <c r="C25" s="13" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D25" s="13"/>
       <c r="E25" s="13"/>
@@ -3442,7 +3704,7 @@
         <v>2</v>
       </c>
       <c r="M25" s="13" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="N25" s="13"/>
       <c r="O25" s="13"/>
@@ -3450,11 +3712,65 @@
       <c r="Q25" s="13"/>
       <c r="R25" s="13"/>
       <c r="S25" s="13"/>
-    </row>
-    <row r="26" spans="2:19">
+      <c r="X25" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y25" s="18"/>
+      <c r="Z25" s="18"/>
+      <c r="AA25" s="18"/>
+      <c r="AB25" s="18"/>
+      <c r="AC25" s="18"/>
+      <c r="AD25" s="18"/>
+      <c r="AE25" s="18"/>
+      <c r="AF25" s="18"/>
+      <c r="AG25" s="18"/>
+      <c r="AH25" s="18"/>
+      <c r="AI25" s="18"/>
+      <c r="AJ25" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK25" s="18"/>
+      <c r="AL25" s="18"/>
+      <c r="AM25" s="18"/>
+      <c r="AN25" s="18"/>
+      <c r="AO25" s="18"/>
+      <c r="AP25" s="18"/>
+      <c r="AQ25" s="18"/>
+      <c r="AR25" s="18"/>
+      <c r="AS25" s="18"/>
+      <c r="AT25" s="18"/>
+      <c r="AU25" s="18"/>
+      <c r="AV25" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="AW25" s="18"/>
+      <c r="AX25" s="18"/>
+      <c r="AY25" s="18"/>
+      <c r="AZ25" s="18"/>
+      <c r="BA25" s="18"/>
+      <c r="BB25" s="18"/>
+      <c r="BC25" s="18"/>
+      <c r="BD25" s="18"/>
+      <c r="BE25" s="18"/>
+      <c r="BF25" s="18"/>
+      <c r="BG25" s="18"/>
+      <c r="BH25" s="18"/>
+      <c r="BI25" s="18"/>
+      <c r="BJ25" s="18"/>
+      <c r="BK25" s="18"/>
+      <c r="BL25" s="18"/>
+      <c r="BM25" s="18"/>
+      <c r="BN25" s="18"/>
+      <c r="BO25" s="18"/>
+      <c r="BP25" s="18"/>
+      <c r="BQ25" s="18"/>
+      <c r="BR25" s="18"/>
+      <c r="BS25" s="18"/>
+    </row>
+    <row r="26" spans="2:71">
       <c r="B26" s="17"/>
       <c r="C26" s="13" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
@@ -3465,10 +3781,10 @@
       <c r="J26" s="13"/>
       <c r="K26" s="13"/>
       <c r="L26" s="13" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="M26" s="13" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="N26" s="13"/>
       <c r="O26" s="13"/>
@@ -3476,13 +3792,67 @@
       <c r="Q26" s="13"/>
       <c r="R26" s="13"/>
       <c r="S26" s="13"/>
-    </row>
-    <row r="27" spans="2:19">
+      <c r="X26" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y26" s="18"/>
+      <c r="Z26" s="18"/>
+      <c r="AA26" s="18"/>
+      <c r="AB26" s="18"/>
+      <c r="AC26" s="18"/>
+      <c r="AD26" s="18"/>
+      <c r="AE26" s="18"/>
+      <c r="AF26" s="18"/>
+      <c r="AG26" s="18"/>
+      <c r="AH26" s="18"/>
+      <c r="AI26" s="18"/>
+      <c r="AJ26" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="AK26" s="18"/>
+      <c r="AL26" s="18"/>
+      <c r="AM26" s="18"/>
+      <c r="AN26" s="18"/>
+      <c r="AO26" s="18"/>
+      <c r="AP26" s="18"/>
+      <c r="AQ26" s="18"/>
+      <c r="AR26" s="18"/>
+      <c r="AS26" s="18"/>
+      <c r="AT26" s="18"/>
+      <c r="AU26" s="18"/>
+      <c r="AV26" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="AW26" s="18"/>
+      <c r="AX26" s="18"/>
+      <c r="AY26" s="18"/>
+      <c r="AZ26" s="18"/>
+      <c r="BA26" s="18"/>
+      <c r="BB26" s="18"/>
+      <c r="BC26" s="18"/>
+      <c r="BD26" s="18"/>
+      <c r="BE26" s="18"/>
+      <c r="BF26" s="18"/>
+      <c r="BG26" s="18"/>
+      <c r="BH26" s="18"/>
+      <c r="BI26" s="18"/>
+      <c r="BJ26" s="18"/>
+      <c r="BK26" s="18"/>
+      <c r="BL26" s="18"/>
+      <c r="BM26" s="18"/>
+      <c r="BN26" s="18"/>
+      <c r="BO26" s="18"/>
+      <c r="BP26" s="18"/>
+      <c r="BQ26" s="18"/>
+      <c r="BR26" s="18"/>
+      <c r="BS26" s="18"/>
+    </row>
+    <row r="27" spans="2:71">
       <c r="B27" s="13" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="13"/>
@@ -3496,7 +3866,7 @@
         <v>6</v>
       </c>
       <c r="M27" s="13" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="N27" s="13"/>
       <c r="O27" s="13"/>
@@ -3504,13 +3874,67 @@
       <c r="Q27" s="13"/>
       <c r="R27" s="13"/>
       <c r="S27" s="13"/>
-    </row>
-    <row r="28" spans="2:19">
+      <c r="X27" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y27" s="18"/>
+      <c r="Z27" s="18"/>
+      <c r="AA27" s="18"/>
+      <c r="AB27" s="18"/>
+      <c r="AC27" s="18"/>
+      <c r="AD27" s="18"/>
+      <c r="AE27" s="18"/>
+      <c r="AF27" s="18"/>
+      <c r="AG27" s="18"/>
+      <c r="AH27" s="18"/>
+      <c r="AI27" s="18"/>
+      <c r="AJ27" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="AK27" s="18"/>
+      <c r="AL27" s="18"/>
+      <c r="AM27" s="18"/>
+      <c r="AN27" s="18"/>
+      <c r="AO27" s="18"/>
+      <c r="AP27" s="18"/>
+      <c r="AQ27" s="18"/>
+      <c r="AR27" s="18"/>
+      <c r="AS27" s="18"/>
+      <c r="AT27" s="18"/>
+      <c r="AU27" s="18"/>
+      <c r="AV27" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AW27" s="18"/>
+      <c r="AX27" s="18"/>
+      <c r="AY27" s="18"/>
+      <c r="AZ27" s="18"/>
+      <c r="BA27" s="18"/>
+      <c r="BB27" s="18"/>
+      <c r="BC27" s="18"/>
+      <c r="BD27" s="18"/>
+      <c r="BE27" s="18"/>
+      <c r="BF27" s="18"/>
+      <c r="BG27" s="18"/>
+      <c r="BH27" s="18"/>
+      <c r="BI27" s="18"/>
+      <c r="BJ27" s="18"/>
+      <c r="BK27" s="18"/>
+      <c r="BL27" s="18"/>
+      <c r="BM27" s="18"/>
+      <c r="BN27" s="18"/>
+      <c r="BO27" s="18"/>
+      <c r="BP27" s="18"/>
+      <c r="BQ27" s="18"/>
+      <c r="BR27" s="18"/>
+      <c r="BS27" s="18"/>
+    </row>
+    <row r="28" spans="2:71">
       <c r="B28" s="13" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="D28" s="13"/>
       <c r="E28" s="13"/>
@@ -3528,13 +3952,67 @@
       <c r="Q28" s="13"/>
       <c r="R28" s="13"/>
       <c r="S28" s="13"/>
-    </row>
-    <row r="29" spans="2:19">
+      <c r="X28" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y28" s="18"/>
+      <c r="Z28" s="18"/>
+      <c r="AA28" s="18"/>
+      <c r="AB28" s="18"/>
+      <c r="AC28" s="18"/>
+      <c r="AD28" s="18"/>
+      <c r="AE28" s="18"/>
+      <c r="AF28" s="18"/>
+      <c r="AG28" s="18"/>
+      <c r="AH28" s="18"/>
+      <c r="AI28" s="18"/>
+      <c r="AJ28" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="AK28" s="18"/>
+      <c r="AL28" s="18"/>
+      <c r="AM28" s="18"/>
+      <c r="AN28" s="18"/>
+      <c r="AO28" s="18"/>
+      <c r="AP28" s="18"/>
+      <c r="AQ28" s="18"/>
+      <c r="AR28" s="18"/>
+      <c r="AS28" s="18"/>
+      <c r="AT28" s="18"/>
+      <c r="AU28" s="18"/>
+      <c r="AV28" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="AW28" s="18"/>
+      <c r="AX28" s="18"/>
+      <c r="AY28" s="18"/>
+      <c r="AZ28" s="18"/>
+      <c r="BA28" s="18"/>
+      <c r="BB28" s="18"/>
+      <c r="BC28" s="18"/>
+      <c r="BD28" s="18"/>
+      <c r="BE28" s="18"/>
+      <c r="BF28" s="18"/>
+      <c r="BG28" s="18"/>
+      <c r="BH28" s="18"/>
+      <c r="BI28" s="18"/>
+      <c r="BJ28" s="18"/>
+      <c r="BK28" s="18"/>
+      <c r="BL28" s="18"/>
+      <c r="BM28" s="18"/>
+      <c r="BN28" s="18"/>
+      <c r="BO28" s="18"/>
+      <c r="BP28" s="18"/>
+      <c r="BQ28" s="18"/>
+      <c r="BR28" s="18"/>
+      <c r="BS28" s="18"/>
+    </row>
+    <row r="29" spans="2:71">
       <c r="B29" s="13" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>26</v>
+        <v>47</v>
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
@@ -3552,8 +4030,62 @@
       <c r="Q29" s="13"/>
       <c r="R29" s="13"/>
       <c r="S29" s="13"/>
-    </row>
-    <row r="30" spans="2:19">
+      <c r="X29" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y29" s="18"/>
+      <c r="Z29" s="18"/>
+      <c r="AA29" s="18"/>
+      <c r="AB29" s="18"/>
+      <c r="AC29" s="18"/>
+      <c r="AD29" s="18"/>
+      <c r="AE29" s="18"/>
+      <c r="AF29" s="18"/>
+      <c r="AG29" s="18"/>
+      <c r="AH29" s="18"/>
+      <c r="AI29" s="18"/>
+      <c r="AJ29" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK29" s="18"/>
+      <c r="AL29" s="18"/>
+      <c r="AM29" s="18"/>
+      <c r="AN29" s="18"/>
+      <c r="AO29" s="18"/>
+      <c r="AP29" s="18"/>
+      <c r="AQ29" s="18"/>
+      <c r="AR29" s="18"/>
+      <c r="AS29" s="18"/>
+      <c r="AT29" s="18"/>
+      <c r="AU29" s="18"/>
+      <c r="AV29" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="AW29" s="18"/>
+      <c r="AX29" s="18"/>
+      <c r="AY29" s="18"/>
+      <c r="AZ29" s="18"/>
+      <c r="BA29" s="18"/>
+      <c r="BB29" s="18"/>
+      <c r="BC29" s="18"/>
+      <c r="BD29" s="18"/>
+      <c r="BE29" s="18"/>
+      <c r="BF29" s="18"/>
+      <c r="BG29" s="18"/>
+      <c r="BH29" s="18"/>
+      <c r="BI29" s="18"/>
+      <c r="BJ29" s="18"/>
+      <c r="BK29" s="18"/>
+      <c r="BL29" s="18"/>
+      <c r="BM29" s="18"/>
+      <c r="BN29" s="18"/>
+      <c r="BO29" s="18"/>
+      <c r="BP29" s="18"/>
+      <c r="BQ29" s="18"/>
+      <c r="BR29" s="18"/>
+      <c r="BS29" s="18"/>
+    </row>
+    <row r="30" spans="2:71">
       <c r="B30" s="14"/>
       <c r="C30" s="14"/>
       <c r="D30" s="14"/>
@@ -3572,6 +4104,60 @@
       <c r="Q30" s="13"/>
       <c r="R30" s="13"/>
       <c r="S30" s="13"/>
+      <c r="X30" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y30" s="18"/>
+      <c r="Z30" s="18"/>
+      <c r="AA30" s="18"/>
+      <c r="AB30" s="18"/>
+      <c r="AC30" s="18"/>
+      <c r="AD30" s="18"/>
+      <c r="AE30" s="18"/>
+      <c r="AF30" s="18"/>
+      <c r="AG30" s="18"/>
+      <c r="AH30" s="18"/>
+      <c r="AI30" s="18"/>
+      <c r="AJ30" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="AK30" s="18"/>
+      <c r="AL30" s="18"/>
+      <c r="AM30" s="18"/>
+      <c r="AN30" s="18"/>
+      <c r="AO30" s="18"/>
+      <c r="AP30" s="18"/>
+      <c r="AQ30" s="18"/>
+      <c r="AR30" s="18"/>
+      <c r="AS30" s="18"/>
+      <c r="AT30" s="18"/>
+      <c r="AU30" s="18"/>
+      <c r="AV30" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="AW30" s="18"/>
+      <c r="AX30" s="18"/>
+      <c r="AY30" s="18"/>
+      <c r="AZ30" s="18"/>
+      <c r="BA30" s="18"/>
+      <c r="BB30" s="18"/>
+      <c r="BC30" s="18"/>
+      <c r="BD30" s="18"/>
+      <c r="BE30" s="18"/>
+      <c r="BF30" s="18"/>
+      <c r="BG30" s="18"/>
+      <c r="BH30" s="18"/>
+      <c r="BI30" s="18"/>
+      <c r="BJ30" s="18"/>
+      <c r="BK30" s="18"/>
+      <c r="BL30" s="18"/>
+      <c r="BM30" s="18"/>
+      <c r="BN30" s="18"/>
+      <c r="BO30" s="18"/>
+      <c r="BP30" s="18"/>
+      <c r="BQ30" s="18"/>
+      <c r="BR30" s="18"/>
+      <c r="BS30" s="18"/>
     </row>
     <row r="31" spans="3:3">
       <c r="C31" s="9"/>
@@ -3679,10 +4265,48 @@
       <c r="C65" s="9"/>
     </row>
   </sheetData>
+  <mergeCells count="36">
+    <mergeCell ref="X22:AI22"/>
+    <mergeCell ref="AJ22:AU22"/>
+    <mergeCell ref="AV22:BG22"/>
+    <mergeCell ref="BH22:BS22"/>
+    <mergeCell ref="X23:AI23"/>
+    <mergeCell ref="AJ23:AU23"/>
+    <mergeCell ref="AV23:BG23"/>
+    <mergeCell ref="BH23:BS23"/>
+    <mergeCell ref="X24:AI24"/>
+    <mergeCell ref="AJ24:AU24"/>
+    <mergeCell ref="AV24:BG24"/>
+    <mergeCell ref="BH24:BS24"/>
+    <mergeCell ref="X25:AI25"/>
+    <mergeCell ref="AJ25:AU25"/>
+    <mergeCell ref="AV25:BG25"/>
+    <mergeCell ref="BH25:BS25"/>
+    <mergeCell ref="X26:AI26"/>
+    <mergeCell ref="AJ26:AU26"/>
+    <mergeCell ref="AV26:BG26"/>
+    <mergeCell ref="BH26:BS26"/>
+    <mergeCell ref="X27:AI27"/>
+    <mergeCell ref="AJ27:AU27"/>
+    <mergeCell ref="AV27:BG27"/>
+    <mergeCell ref="BH27:BS27"/>
+    <mergeCell ref="X28:AI28"/>
+    <mergeCell ref="AJ28:AU28"/>
+    <mergeCell ref="AV28:BG28"/>
+    <mergeCell ref="BH28:BS28"/>
+    <mergeCell ref="X29:AI29"/>
+    <mergeCell ref="AJ29:AU29"/>
+    <mergeCell ref="AV29:BG29"/>
+    <mergeCell ref="BH29:BS29"/>
+    <mergeCell ref="X30:AI30"/>
+    <mergeCell ref="AJ30:AU30"/>
+    <mergeCell ref="AV30:BG30"/>
+    <mergeCell ref="BH30:BS30"/>
+  </mergeCells>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1585986283" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1586161829" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -3691,16 +4315,16 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1585986283" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1585986283" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1585986283" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1585986283" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1586161829" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1586161829" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1586161829" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1586161829" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1585986283" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1586161829" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>

<commit_message>
Needs LORE, WEAPON and COMBAT
</commit_message>
<xml_diff>
--- a/template mapas.xlsx
+++ b/template mapas.xlsx
@@ -5,25 +5,26 @@
   <fileSharing readOnlyRecommended="0" userName="alexm"/>
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
+    <workbookView activeTab="1" xWindow="240" yWindow="60" windowWidth="0" windowHeight="0" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId4"/>
+    <sheet name="Map01" sheetId="1" r:id="rId4"/>
+    <sheet name="Map02" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1586161829" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1586161829" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1586161829" overlapCells="1"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1586161829"/>
+      <pm:revision xmlns:pm="smNativeData" day="1586327817" val="976" rev="124" revOS="4" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1586327817" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1586327817" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1586327817"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="87">
   <si>
     <t>x</t>
   </si>
@@ -185,6 +186,105 @@
   </si>
   <si>
     <t>map01[11][54] = ENEMY;</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>map02[3][51] = ENEMY;</t>
+  </si>
+  <si>
+    <t>map02[12][24] = ENEMY;</t>
+  </si>
+  <si>
+    <t>map02[6][25] = LEVER_ON;</t>
+  </si>
+  <si>
+    <t>map02[7][15] = BARRIER;</t>
+  </si>
+  <si>
+    <t>map02[17][53] = ENEMY;</t>
+  </si>
+  <si>
+    <t>map02[5][18] = ENEMY;</t>
+  </si>
+  <si>
+    <t>map02[9][44] = POTION;</t>
+  </si>
+  <si>
+    <t>map02[2][16] = WEAPON;</t>
+  </si>
+  <si>
+    <t>map02[6][40] = ENEMY;</t>
+  </si>
+  <si>
+    <t>map02[2][44] = KEY;</t>
+  </si>
+  <si>
+    <t>map02[18][27] = POTION;</t>
+  </si>
+  <si>
+    <t>map02[7][14] = NPC;</t>
+  </si>
+  <si>
+    <t>map02[3][35] = ENEMY;</t>
+  </si>
+  <si>
+    <t>map02[18][35] = KEY;</t>
+  </si>
+  <si>
+    <t>map02[17][43] = V_DOOR;</t>
+  </si>
+  <si>
+    <t>map02[17][40] = ENEMY;</t>
+  </si>
+  <si>
+    <t>map02[7][22] = KEY;</t>
+  </si>
+  <si>
+    <t>map02[17][21] = V_DOOR;</t>
+  </si>
+  <si>
+    <t>map02[12][35] = ENEMY;</t>
+  </si>
+  <si>
+    <t>map02[7][55] = LEVER_ON;</t>
+  </si>
+  <si>
+    <t>map02[4][26] = V_DOOR;</t>
+  </si>
+  <si>
+    <t>NPC</t>
+  </si>
+  <si>
+    <t>map02[9][34] = ENEMY;</t>
+  </si>
+  <si>
+    <t>map02[17][36] = LEVER_ON;</t>
+  </si>
+  <si>
+    <t>map02[10][46] = BARRIER;</t>
+  </si>
+  <si>
+    <t>map02[6][29] = ENEMY;</t>
+  </si>
+  <si>
+    <t>map02[1][27] = LEVER_ON;</t>
+  </si>
+  <si>
+    <t>map02[16][35] = BARRIER;</t>
+  </si>
+  <si>
+    <t>map02[15][29] = ENEMY;</t>
+  </si>
+  <si>
+    <t>map02[1][23] = LEVER_ON;</t>
+  </si>
+  <si>
+    <t>map02[15][26] = BARRIER;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -209,7 +309,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1586161829" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1586327817" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -225,7 +325,7 @@
       <sz val="20"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1586161829" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1586327817" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="400" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -241,7 +341,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1586161829" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1586327817" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -257,7 +357,7 @@
       <sz val="16"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1586161829" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1586327817" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="320" lang="default" weight="bold"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -266,7 +366,7 @@
       </extLst>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,7 +379,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586327817" type="1" fgLvl="38" fgClr="00FFFF00" bgLvl="62" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -290,7 +390,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="71" fgClr="00FFFFFF" bgLvl="29" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586327817" type="1" fgLvl="71" fgClr="00FFFFFF" bgLvl="29" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -301,7 +401,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="0" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586327817" type="1" fgLvl="0" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -312,7 +412,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="100" fgClr="004D4D4D" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586327817" type="1" fgLvl="100" fgClr="004D4D4D" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -323,7 +423,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="100" fgClr="00B3B3B3" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586327817" type="1" fgLvl="100" fgClr="00B3B3B3" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -334,7 +434,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="100" fgClr="007F7F7F" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586327817" type="1" fgLvl="100" fgClr="007F7F7F" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -345,7 +445,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="100" fgClr="00000000" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586327817" type="1" fgLvl="100" fgClr="00000000" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -356,7 +456,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586327817" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -367,7 +467,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586327817" type="1" fgLvl="100" fgClr="00E6E6E6" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
@@ -378,13 +478,24 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1586161829" type="1" fgLvl="100" fgClr="00333333" bgLvl="0" bgClr="00FFFFFF"/>
+            <pm:shade xmlns:pm="smNativeData" id="1586327817" type="1" fgLvl="100" fgClr="00333333" bgLvl="0" bgClr="00FFFFFF"/>
+          </ext>
+        </extLst>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+        <extLst>
+          <ext uri="smNativeData">
+            <pm:shade xmlns:pm="smNativeData" id="1586327817" type="1" fgLvl="100" fgClr="00CCCCCC" bgLvl="0" bgClr="00FFFFFF"/>
           </ext>
         </extLst>
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left style="none">
         <color rgb="FF000000"/>
@@ -400,7 +511,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
+          <pm:border xmlns:pm="smNativeData" id="1586327817"/>
         </ext>
       </extLst>
     </border>
@@ -419,7 +530,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
+          <pm:border xmlns:pm="smNativeData" id="1586327817"/>
         </ext>
       </extLst>
     </border>
@@ -438,7 +549,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
+          <pm:border xmlns:pm="smNativeData" id="1586327817"/>
         </ext>
       </extLst>
     </border>
@@ -457,7 +568,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
+          <pm:border xmlns:pm="smNativeData" id="1586327817"/>
         </ext>
       </extLst>
     </border>
@@ -476,7 +587,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
+          <pm:border xmlns:pm="smNativeData" id="1586327817"/>
         </ext>
       </extLst>
     </border>
@@ -495,7 +606,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
+          <pm:border xmlns:pm="smNativeData" id="1586327817"/>
         </ext>
       </extLst>
     </border>
@@ -514,7 +625,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
+          <pm:border xmlns:pm="smNativeData" id="1586327817"/>
         </ext>
       </extLst>
     </border>
@@ -533,7 +644,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
+          <pm:border xmlns:pm="smNativeData" id="1586327817"/>
         </ext>
       </extLst>
     </border>
@@ -552,7 +663,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
+          <pm:border xmlns:pm="smNativeData" id="1586327817"/>
         </ext>
       </extLst>
     </border>
@@ -571,7 +682,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
+          <pm:border xmlns:pm="smNativeData" id="1586327817"/>
         </ext>
       </extLst>
     </border>
@@ -590,7 +701,26 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1586161829"/>
+          <pm:border xmlns:pm="smNativeData" id="1586327817"/>
+        </ext>
+      </extLst>
+    </border>
+    <border>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:border xmlns:pm="smNativeData" id="1586327817"/>
         </ext>
       </extLst>
     </border>
@@ -661,10 +791,10 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1586161829" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1586327817" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
-      <pm:colors xmlns:pm="smNativeData" id="1586161829" count="4">
+      <pm:colors xmlns:pm="smNativeData" id="1586327817" count="4">
         <pm:color name="Cor 24" rgb="FFFF9E"/>
         <pm:color name="Cor 25" rgb="B5B5B5"/>
         <pm:color name="Cor 26" rgb="6B6B6B"/>
@@ -933,7 +1063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:CZ65"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" zoomScale="60" workbookViewId="0">
+    <sheetView view="normal" topLeftCell="A10" zoomScale="60" workbookViewId="0">
       <selection activeCell="X22" sqref="X22:AI22"/>
     </sheetView>
   </sheetViews>
@@ -4306,7 +4436,7 @@
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1586161829" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1586327817" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -4315,16 +4445,3433 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1586161829" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1586161829" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1586161829" Id="0" type="0" value="0"/>
-        <pm:paperBin xmlns:pm="smNativeData" id="1586161829" Id="1" type="0" value="0"/>
+        <pm:header xmlns:pm="smNativeData" id="1586327817" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1586327817" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1586327817" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1586327817" Id="1" type="0" value="0"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1586161829" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1586327817" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+        <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+        <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
+      </pm:sheetPrefs>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:CZ65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="normal" zoomScale="80" workbookViewId="0">
+      <selection activeCell="BH22" sqref="BH22:BS24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="24.95"/>
+  <cols>
+    <col min="1" max="1" width="10.000000" style="1"/>
+    <col min="2" max="63" width="3.828829" customWidth="1" style="2"/>
+    <col min="64" max="64" width="4.810811" customWidth="1" style="2"/>
+    <col min="65" max="104" width="3.828829" customWidth="1" style="2"/>
+    <col min="105" max="16384" width="10.000000" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:104" s="3" customFormat="1" ht="23.85" customHeight="1">
+      <c r="B1" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="I1" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="J1" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="K1" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="L1" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="M1" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="N1" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="O1" s="3" t="n">
+        <v>13</v>
+      </c>
+      <c r="P1" s="3" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="R1" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="S1" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="T1" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="U1" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="V1" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="W1" s="3" t="n">
+        <v>21</v>
+      </c>
+      <c r="X1" s="3" t="n">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="3" t="n">
+        <v>23</v>
+      </c>
+      <c r="Z1" s="3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA1" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="3" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC1" s="3" t="n">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="3" t="n">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="3" t="n">
+        <v>29</v>
+      </c>
+      <c r="AF1" s="3" t="n">
+        <v>30</v>
+      </c>
+      <c r="AG1" s="3" t="n">
+        <v>31</v>
+      </c>
+      <c r="AH1" s="3" t="n">
+        <v>32</v>
+      </c>
+      <c r="AI1" s="3" t="n">
+        <v>33</v>
+      </c>
+      <c r="AJ1" s="3" t="n">
+        <v>34</v>
+      </c>
+      <c r="AK1" s="3" t="n">
+        <v>35</v>
+      </c>
+      <c r="AL1" s="3" t="n">
+        <v>36</v>
+      </c>
+      <c r="AM1" s="3" t="n">
+        <v>37</v>
+      </c>
+      <c r="AN1" s="3" t="n">
+        <v>38</v>
+      </c>
+      <c r="AO1" s="3" t="n">
+        <v>39</v>
+      </c>
+      <c r="AP1" s="3" t="n">
+        <v>40</v>
+      </c>
+      <c r="AQ1" s="3" t="n">
+        <v>41</v>
+      </c>
+      <c r="AR1" s="3" t="n">
+        <v>42</v>
+      </c>
+      <c r="AS1" s="3" t="n">
+        <v>43</v>
+      </c>
+      <c r="AT1" s="3" t="n">
+        <v>44</v>
+      </c>
+      <c r="AU1" s="3" t="n">
+        <v>45</v>
+      </c>
+      <c r="AV1" s="3" t="n">
+        <v>46</v>
+      </c>
+      <c r="AW1" s="3" t="n">
+        <v>47</v>
+      </c>
+      <c r="AX1" s="3" t="n">
+        <v>48</v>
+      </c>
+      <c r="AY1" s="3" t="n">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="3" t="n">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="3" t="n">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="3" t="n">
+        <v>52</v>
+      </c>
+      <c r="BC1" s="3" t="n">
+        <v>53</v>
+      </c>
+      <c r="BD1" s="3" t="n">
+        <v>54</v>
+      </c>
+      <c r="BE1" s="3" t="n">
+        <v>55</v>
+      </c>
+      <c r="BF1" s="3" t="n">
+        <v>56</v>
+      </c>
+      <c r="BG1" s="3" t="n">
+        <v>57</v>
+      </c>
+      <c r="BH1" s="3" t="n">
+        <v>58</v>
+      </c>
+      <c r="BI1" s="3" t="n">
+        <v>59</v>
+      </c>
+      <c r="BJ1" s="3" t="n">
+        <v>60</v>
+      </c>
+      <c r="BK1" s="3" t="n">
+        <v>61</v>
+      </c>
+      <c r="BL1" s="11"/>
+      <c r="BM1" s="11"/>
+      <c r="BN1" s="11"/>
+      <c r="BO1" s="11"/>
+      <c r="BP1" s="11"/>
+      <c r="BQ1" s="11"/>
+      <c r="BR1" s="11"/>
+      <c r="BS1" s="11"/>
+      <c r="BT1" s="11"/>
+      <c r="BU1" s="11"/>
+      <c r="BV1" s="11"/>
+      <c r="BW1" s="11"/>
+      <c r="BX1" s="11"/>
+      <c r="BY1" s="11"/>
+      <c r="BZ1" s="11"/>
+      <c r="CA1" s="11"/>
+      <c r="CB1" s="11"/>
+      <c r="CC1" s="11"/>
+      <c r="CD1" s="11"/>
+      <c r="CE1" s="11"/>
+      <c r="CF1" s="11"/>
+      <c r="CG1" s="11"/>
+      <c r="CH1" s="11"/>
+      <c r="CI1" s="11"/>
+      <c r="CJ1" s="11"/>
+      <c r="CK1" s="11"/>
+      <c r="CL1" s="11"/>
+      <c r="CM1" s="11"/>
+      <c r="CN1" s="11"/>
+      <c r="CO1" s="11"/>
+      <c r="CP1" s="11"/>
+      <c r="CQ1" s="11"/>
+      <c r="CR1" s="11"/>
+      <c r="CS1" s="11"/>
+      <c r="CT1" s="11"/>
+      <c r="CU1" s="11"/>
+      <c r="CV1" s="11"/>
+      <c r="CW1" s="11"/>
+      <c r="CX1" s="11"/>
+      <c r="CY1" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="CZ1" s="3" t="n">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="10"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5"/>
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="10"/>
+      <c r="AQ2" s="10"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" s="10"/>
+      <c r="AT2" s="10"/>
+      <c r="AU2" s="10"/>
+      <c r="AV2" s="10"/>
+      <c r="AW2" s="10"/>
+      <c r="AX2" s="10"/>
+      <c r="AY2" s="10"/>
+      <c r="AZ2" s="10"/>
+      <c r="BA2" s="10"/>
+      <c r="BB2" s="10"/>
+      <c r="BC2" s="10"/>
+      <c r="BD2" s="10"/>
+      <c r="BE2" s="10"/>
+      <c r="BF2" s="10"/>
+      <c r="BG2" s="10"/>
+      <c r="BH2" s="10"/>
+      <c r="BI2" s="10"/>
+      <c r="BJ2" s="10"/>
+      <c r="BK2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL2" s="12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM2" s="12"/>
+      <c r="BN2" s="12"/>
+      <c r="BO2" s="12"/>
+      <c r="BP2" s="12"/>
+      <c r="BQ2" s="12"/>
+      <c r="BR2" s="12"/>
+      <c r="BS2" s="12"/>
+      <c r="BT2" s="12"/>
+      <c r="BU2" s="12"/>
+      <c r="BV2" s="12"/>
+      <c r="BW2" s="12"/>
+      <c r="BX2" s="12"/>
+      <c r="BY2" s="12"/>
+      <c r="BZ2" s="12"/>
+      <c r="CA2" s="12"/>
+      <c r="CB2" s="12"/>
+      <c r="CC2" s="12"/>
+      <c r="CD2" s="12"/>
+      <c r="CE2" s="12"/>
+      <c r="CF2" s="12"/>
+      <c r="CG2" s="12"/>
+      <c r="CH2" s="12"/>
+      <c r="CI2" s="12"/>
+      <c r="CJ2" s="12"/>
+      <c r="CK2" s="12"/>
+      <c r="CL2" s="12"/>
+      <c r="CM2" s="12"/>
+      <c r="CN2" s="12"/>
+      <c r="CO2" s="12"/>
+      <c r="CP2" s="12"/>
+      <c r="CQ2" s="12"/>
+      <c r="CR2" s="12"/>
+      <c r="CS2" s="12"/>
+      <c r="CT2" s="12"/>
+      <c r="CU2" s="12"/>
+      <c r="CV2" s="12"/>
+      <c r="CW2" s="12"/>
+      <c r="CX2" s="12"/>
+    </row>
+    <row r="3" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="6"/>
+      <c r="AC3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="8"/>
+      <c r="AL3" s="8"/>
+      <c r="AM3" s="8"/>
+      <c r="AN3" s="8"/>
+      <c r="AO3" s="8"/>
+      <c r="AP3" s="8"/>
+      <c r="AQ3" s="8"/>
+      <c r="AR3" s="8"/>
+      <c r="AS3" s="6"/>
+      <c r="AT3" s="8"/>
+      <c r="AU3" s="8"/>
+      <c r="AV3" s="8"/>
+      <c r="AW3" s="6"/>
+      <c r="AX3" s="8"/>
+      <c r="AY3" s="8"/>
+      <c r="AZ3" s="8"/>
+      <c r="BA3" s="8"/>
+      <c r="BB3" s="8"/>
+      <c r="BC3" s="8"/>
+      <c r="BD3" s="8"/>
+      <c r="BE3" s="8"/>
+      <c r="BF3" s="8"/>
+      <c r="BG3" s="8"/>
+      <c r="BH3" s="8"/>
+      <c r="BI3" s="8"/>
+      <c r="BJ3" s="5"/>
+      <c r="BK3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL3" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM3" s="12"/>
+      <c r="BN3" s="12"/>
+      <c r="BO3" s="12"/>
+      <c r="BP3" s="12"/>
+      <c r="BQ3" s="12"/>
+      <c r="BR3" s="12"/>
+      <c r="BS3" s="12"/>
+      <c r="BT3" s="12"/>
+      <c r="BU3" s="12"/>
+      <c r="BV3" s="12"/>
+      <c r="BW3" s="12"/>
+      <c r="BX3" s="12"/>
+      <c r="BY3" s="12"/>
+      <c r="BZ3" s="12"/>
+      <c r="CA3" s="12"/>
+      <c r="CB3" s="12"/>
+      <c r="CC3" s="12"/>
+      <c r="CD3" s="12"/>
+      <c r="CE3" s="12"/>
+      <c r="CF3" s="12"/>
+      <c r="CG3" s="12"/>
+      <c r="CH3" s="12"/>
+      <c r="CI3" s="12"/>
+      <c r="CJ3" s="12"/>
+      <c r="CK3" s="12"/>
+      <c r="CL3" s="12"/>
+      <c r="CM3" s="12"/>
+      <c r="CN3" s="12"/>
+      <c r="CO3" s="12"/>
+      <c r="CP3" s="12"/>
+      <c r="CQ3" s="12"/>
+      <c r="CR3" s="12"/>
+      <c r="CS3" s="12"/>
+      <c r="CT3" s="12"/>
+      <c r="CU3" s="12"/>
+      <c r="CV3" s="12"/>
+      <c r="CW3" s="12"/>
+      <c r="CX3" s="12"/>
+    </row>
+    <row r="4" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="7"/>
+      <c r="AD4" s="7"/>
+      <c r="AE4" s="7"/>
+      <c r="AF4" s="7"/>
+      <c r="AG4" s="7"/>
+      <c r="AH4" s="7"/>
+      <c r="AI4" s="7"/>
+      <c r="AJ4" s="7"/>
+      <c r="AK4" s="7"/>
+      <c r="AL4" s="7"/>
+      <c r="AM4" s="7"/>
+      <c r="AN4" s="7"/>
+      <c r="AO4" s="7"/>
+      <c r="AP4" s="7"/>
+      <c r="AQ4" s="7"/>
+      <c r="AR4" s="7"/>
+      <c r="AS4" s="6"/>
+      <c r="AT4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU4" s="7"/>
+      <c r="AV4" s="7"/>
+      <c r="AW4" s="8"/>
+      <c r="AX4" s="7"/>
+      <c r="AY4" s="7"/>
+      <c r="AZ4" s="7"/>
+      <c r="BA4" s="7"/>
+      <c r="BB4" s="7"/>
+      <c r="BC4" s="7"/>
+      <c r="BD4" s="7"/>
+      <c r="BE4" s="7"/>
+      <c r="BF4" s="7"/>
+      <c r="BG4" s="7"/>
+      <c r="BH4" s="7"/>
+      <c r="BI4" s="7"/>
+      <c r="BJ4" s="5"/>
+      <c r="BK4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL4" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="BM4" s="12"/>
+      <c r="BN4" s="12"/>
+      <c r="BO4" s="12"/>
+      <c r="BP4" s="12"/>
+      <c r="BQ4" s="12"/>
+      <c r="BR4" s="12"/>
+      <c r="BS4" s="12"/>
+      <c r="BT4" s="12"/>
+      <c r="BU4" s="12"/>
+      <c r="BV4" s="12"/>
+      <c r="BW4" s="12"/>
+      <c r="BX4" s="12"/>
+      <c r="BY4" s="12"/>
+      <c r="BZ4" s="12"/>
+      <c r="CA4" s="12"/>
+      <c r="CB4" s="12"/>
+      <c r="CC4" s="12"/>
+      <c r="CD4" s="12"/>
+      <c r="CE4" s="12"/>
+      <c r="CF4" s="12"/>
+      <c r="CG4" s="12"/>
+      <c r="CH4" s="12"/>
+      <c r="CI4" s="12"/>
+      <c r="CJ4" s="12"/>
+      <c r="CK4" s="12"/>
+      <c r="CL4" s="12"/>
+      <c r="CM4" s="12"/>
+      <c r="CN4" s="12"/>
+      <c r="CO4" s="12"/>
+      <c r="CP4" s="12"/>
+      <c r="CQ4" s="12"/>
+      <c r="CR4" s="12"/>
+      <c r="CS4" s="12"/>
+      <c r="CT4" s="12"/>
+      <c r="CU4" s="12"/>
+      <c r="CV4" s="12"/>
+      <c r="CW4" s="12"/>
+      <c r="CX4" s="12"/>
+    </row>
+    <row r="5" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="7"/>
+      <c r="AD5" s="7"/>
+      <c r="AE5" s="7"/>
+      <c r="AF5" s="7"/>
+      <c r="AG5" s="7"/>
+      <c r="AH5" s="7"/>
+      <c r="AI5" s="7"/>
+      <c r="AJ5" s="7"/>
+      <c r="AK5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL5" s="7"/>
+      <c r="AM5" s="7"/>
+      <c r="AN5" s="7"/>
+      <c r="AO5" s="7"/>
+      <c r="AP5" s="7"/>
+      <c r="AQ5" s="7"/>
+      <c r="AR5" s="7"/>
+      <c r="AS5" s="6"/>
+      <c r="AT5" s="7"/>
+      <c r="AU5" s="7"/>
+      <c r="AV5" s="7"/>
+      <c r="AW5" s="7"/>
+      <c r="AX5" s="7"/>
+      <c r="AY5" s="7"/>
+      <c r="AZ5" s="7"/>
+      <c r="BA5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="BB5" s="7"/>
+      <c r="BC5" s="7"/>
+      <c r="BD5" s="7"/>
+      <c r="BE5" s="7"/>
+      <c r="BF5" s="6"/>
+      <c r="BG5" s="7"/>
+      <c r="BH5" s="7"/>
+      <c r="BI5" s="7"/>
+      <c r="BJ5" s="5"/>
+      <c r="BK5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL5" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="BM5" s="12"/>
+      <c r="BN5" s="12"/>
+      <c r="BO5" s="12"/>
+      <c r="BP5" s="12"/>
+      <c r="BQ5" s="12"/>
+      <c r="BR5" s="12"/>
+      <c r="BS5" s="12"/>
+      <c r="BT5" s="12"/>
+      <c r="BU5" s="12"/>
+      <c r="BV5" s="12"/>
+      <c r="BW5" s="12"/>
+      <c r="BX5" s="12"/>
+      <c r="BY5" s="12"/>
+      <c r="BZ5" s="12"/>
+      <c r="CA5" s="12"/>
+      <c r="CB5" s="12"/>
+      <c r="CC5" s="12"/>
+      <c r="CD5" s="12"/>
+      <c r="CE5" s="12"/>
+      <c r="CF5" s="12"/>
+      <c r="CG5" s="12"/>
+      <c r="CH5" s="12"/>
+      <c r="CI5" s="12"/>
+      <c r="CJ5" s="12"/>
+      <c r="CK5" s="12"/>
+      <c r="CL5" s="12"/>
+      <c r="CM5" s="12"/>
+      <c r="CN5" s="12"/>
+      <c r="CO5" s="12"/>
+      <c r="CP5" s="12"/>
+      <c r="CQ5" s="12"/>
+      <c r="CR5" s="12"/>
+      <c r="CS5" s="12"/>
+      <c r="CT5" s="12"/>
+      <c r="CU5" s="12"/>
+      <c r="CV5" s="12"/>
+      <c r="CW5" s="12"/>
+      <c r="CX5" s="12"/>
+    </row>
+    <row r="6" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
+      <c r="AB6" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="7"/>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="7"/>
+      <c r="AI6" s="7"/>
+      <c r="AJ6" s="7"/>
+      <c r="AK6" s="7"/>
+      <c r="AL6" s="7"/>
+      <c r="AM6" s="7"/>
+      <c r="AN6" s="7"/>
+      <c r="AO6" s="7"/>
+      <c r="AP6" s="6"/>
+      <c r="AQ6" s="7"/>
+      <c r="AR6" s="7"/>
+      <c r="AS6" s="6"/>
+      <c r="AT6" s="7"/>
+      <c r="AU6" s="7"/>
+      <c r="AV6" s="7"/>
+      <c r="AW6" s="6"/>
+      <c r="AX6" s="7"/>
+      <c r="AY6" s="7"/>
+      <c r="AZ6" s="7"/>
+      <c r="BA6" s="7"/>
+      <c r="BB6" s="7"/>
+      <c r="BC6" s="7"/>
+      <c r="BD6" s="7"/>
+      <c r="BE6" s="7"/>
+      <c r="BF6" s="6"/>
+      <c r="BG6" s="7"/>
+      <c r="BH6" s="7"/>
+      <c r="BI6" s="7"/>
+      <c r="BJ6" s="5"/>
+      <c r="BK6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL6" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="BM6" s="12"/>
+      <c r="BN6" s="12"/>
+      <c r="BO6" s="12"/>
+      <c r="BP6" s="12"/>
+      <c r="BQ6" s="12"/>
+      <c r="BR6" s="12"/>
+      <c r="BS6" s="12"/>
+      <c r="BT6" s="12"/>
+      <c r="BU6" s="12"/>
+      <c r="BV6" s="12"/>
+      <c r="BW6" s="12"/>
+      <c r="BX6" s="12"/>
+      <c r="BY6" s="12"/>
+      <c r="BZ6" s="12"/>
+      <c r="CA6" s="12"/>
+      <c r="CB6" s="12"/>
+      <c r="CC6" s="12"/>
+      <c r="CD6" s="12"/>
+      <c r="CE6" s="12"/>
+      <c r="CF6" s="12"/>
+      <c r="CG6" s="12"/>
+      <c r="CH6" s="12"/>
+      <c r="CI6" s="12"/>
+      <c r="CJ6" s="12"/>
+      <c r="CK6" s="12"/>
+      <c r="CL6" s="12"/>
+      <c r="CM6" s="12"/>
+      <c r="CN6" s="12"/>
+      <c r="CO6" s="12"/>
+      <c r="CP6" s="12"/>
+      <c r="CQ6" s="12"/>
+      <c r="CR6" s="12"/>
+      <c r="CS6" s="12"/>
+      <c r="CT6" s="12"/>
+      <c r="CU6" s="12"/>
+      <c r="CV6" s="12"/>
+      <c r="CW6" s="12"/>
+      <c r="CX6" s="12"/>
+    </row>
+    <row r="7" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="7"/>
+      <c r="AD7" s="7"/>
+      <c r="AE7" s="8"/>
+      <c r="AF7" s="7"/>
+      <c r="AG7" s="7"/>
+      <c r="AH7" s="7"/>
+      <c r="AI7" s="7"/>
+      <c r="AJ7" s="7"/>
+      <c r="AK7" s="7"/>
+      <c r="AL7" s="7"/>
+      <c r="AM7" s="7"/>
+      <c r="AN7" s="7"/>
+      <c r="AO7" s="7"/>
+      <c r="AP7" s="8"/>
+      <c r="AQ7" s="7"/>
+      <c r="AR7" s="7"/>
+      <c r="AS7" s="6"/>
+      <c r="AT7" s="7"/>
+      <c r="AU7" s="7"/>
+      <c r="AV7" s="7"/>
+      <c r="AW7" s="6"/>
+      <c r="AX7" s="7"/>
+      <c r="AY7" s="7"/>
+      <c r="AZ7" s="7"/>
+      <c r="BA7" s="7"/>
+      <c r="BB7" s="7"/>
+      <c r="BC7" s="7"/>
+      <c r="BD7" s="7"/>
+      <c r="BE7" s="7"/>
+      <c r="BF7" s="6"/>
+      <c r="BG7" s="7"/>
+      <c r="BH7" s="7"/>
+      <c r="BI7" s="7"/>
+      <c r="BJ7" s="5"/>
+      <c r="BK7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL7" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="BM7" s="12"/>
+      <c r="BN7" s="12"/>
+      <c r="BO7" s="12"/>
+      <c r="BP7" s="12"/>
+      <c r="BQ7" s="12"/>
+      <c r="BR7" s="12"/>
+      <c r="BS7" s="12"/>
+      <c r="BT7" s="12"/>
+      <c r="BU7" s="12"/>
+      <c r="BV7" s="12"/>
+      <c r="BW7" s="12"/>
+      <c r="BX7" s="12"/>
+      <c r="BY7" s="12"/>
+      <c r="BZ7" s="12"/>
+      <c r="CA7" s="12"/>
+      <c r="CB7" s="12"/>
+      <c r="CC7" s="12"/>
+      <c r="CD7" s="12"/>
+      <c r="CE7" s="12"/>
+      <c r="CF7" s="12"/>
+      <c r="CG7" s="12"/>
+      <c r="CH7" s="12"/>
+      <c r="CI7" s="12"/>
+      <c r="CJ7" s="12"/>
+      <c r="CK7" s="12"/>
+      <c r="CL7" s="12"/>
+      <c r="CM7" s="12"/>
+      <c r="CN7" s="12"/>
+      <c r="CO7" s="12"/>
+      <c r="CP7" s="12"/>
+      <c r="CQ7" s="12"/>
+      <c r="CR7" s="12"/>
+      <c r="CS7" s="12"/>
+      <c r="CT7" s="12"/>
+      <c r="CU7" s="12"/>
+      <c r="CV7" s="12"/>
+      <c r="CW7" s="12"/>
+      <c r="CX7" s="12"/>
+    </row>
+    <row r="8" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="7"/>
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF8" s="7"/>
+      <c r="AG8" s="7"/>
+      <c r="AH8" s="7"/>
+      <c r="AI8" s="7"/>
+      <c r="AJ8" s="7"/>
+      <c r="AK8" s="7"/>
+      <c r="AL8" s="7"/>
+      <c r="AM8" s="7"/>
+      <c r="AN8" s="7"/>
+      <c r="AO8" s="7"/>
+      <c r="AP8" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ8" s="7"/>
+      <c r="AR8" s="7"/>
+      <c r="AS8" s="6"/>
+      <c r="AT8" s="7"/>
+      <c r="AU8" s="7"/>
+      <c r="AV8" s="7"/>
+      <c r="AW8" s="6"/>
+      <c r="AX8" s="6"/>
+      <c r="AY8" s="6"/>
+      <c r="AZ8" s="6"/>
+      <c r="BA8" s="6"/>
+      <c r="BB8" s="6"/>
+      <c r="BC8" s="6"/>
+      <c r="BD8" s="6"/>
+      <c r="BE8" s="6"/>
+      <c r="BF8" s="6"/>
+      <c r="BG8" s="7"/>
+      <c r="BH8" s="7"/>
+      <c r="BI8" s="7"/>
+      <c r="BJ8" s="5"/>
+      <c r="BK8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL8" s="12" t="n">
+        <v>6</v>
+      </c>
+      <c r="BM8" s="12"/>
+      <c r="BN8" s="12"/>
+      <c r="BO8" s="12"/>
+      <c r="BP8" s="12"/>
+      <c r="BQ8" s="12"/>
+      <c r="BR8" s="12"/>
+      <c r="BS8" s="12"/>
+      <c r="BT8" s="12"/>
+      <c r="BU8" s="12"/>
+      <c r="BV8" s="12"/>
+      <c r="BW8" s="12"/>
+      <c r="BX8" s="12"/>
+      <c r="BY8" s="12"/>
+      <c r="BZ8" s="12"/>
+      <c r="CA8" s="12"/>
+      <c r="CB8" s="12"/>
+      <c r="CC8" s="12"/>
+      <c r="CD8" s="12"/>
+      <c r="CE8" s="12"/>
+      <c r="CF8" s="12"/>
+      <c r="CG8" s="12"/>
+      <c r="CH8" s="12"/>
+      <c r="CI8" s="12"/>
+      <c r="CJ8" s="12"/>
+      <c r="CK8" s="12"/>
+      <c r="CL8" s="12"/>
+      <c r="CM8" s="12"/>
+      <c r="CN8" s="12"/>
+      <c r="CO8" s="12"/>
+      <c r="CP8" s="12"/>
+      <c r="CQ8" s="12"/>
+      <c r="CR8" s="12"/>
+      <c r="CS8" s="12"/>
+      <c r="CT8" s="12"/>
+      <c r="CU8" s="12"/>
+      <c r="CV8" s="12"/>
+      <c r="CW8" s="12"/>
+      <c r="CX8" s="12"/>
+    </row>
+    <row r="9" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="5"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="7"/>
+      <c r="AD9" s="7"/>
+      <c r="AE9" s="7"/>
+      <c r="AF9" s="7"/>
+      <c r="AG9" s="7"/>
+      <c r="AH9" s="7"/>
+      <c r="AI9" s="7"/>
+      <c r="AJ9" s="7"/>
+      <c r="AK9" s="7"/>
+      <c r="AL9" s="7"/>
+      <c r="AM9" s="7"/>
+      <c r="AN9" s="7"/>
+      <c r="AO9" s="7"/>
+      <c r="AP9" s="7"/>
+      <c r="AQ9" s="7"/>
+      <c r="AR9" s="7"/>
+      <c r="AS9" s="6"/>
+      <c r="AT9" s="7"/>
+      <c r="AU9" s="7"/>
+      <c r="AV9" s="7"/>
+      <c r="AW9" s="8"/>
+      <c r="AX9" s="8"/>
+      <c r="AY9" s="8"/>
+      <c r="AZ9" s="8"/>
+      <c r="BA9" s="8"/>
+      <c r="BB9" s="8"/>
+      <c r="BC9" s="8"/>
+      <c r="BD9" s="8"/>
+      <c r="BE9" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="BF9" s="6"/>
+      <c r="BG9" s="7"/>
+      <c r="BH9" s="7"/>
+      <c r="BI9" s="7"/>
+      <c r="BJ9" s="5"/>
+      <c r="BK9" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL9" s="12" t="n">
+        <v>7</v>
+      </c>
+      <c r="BM9" s="12"/>
+      <c r="BN9" s="12"/>
+      <c r="BO9" s="12"/>
+      <c r="BP9" s="12"/>
+      <c r="BQ9" s="12"/>
+      <c r="BR9" s="12"/>
+      <c r="BS9" s="12"/>
+      <c r="BT9" s="12"/>
+      <c r="BU9" s="12"/>
+      <c r="BV9" s="12"/>
+      <c r="BW9" s="12"/>
+      <c r="BX9" s="12"/>
+      <c r="BY9" s="12"/>
+      <c r="BZ9" s="12"/>
+      <c r="CA9" s="12"/>
+      <c r="CB9" s="12"/>
+      <c r="CC9" s="12"/>
+      <c r="CD9" s="12"/>
+      <c r="CE9" s="12"/>
+      <c r="CF9" s="12"/>
+      <c r="CG9" s="12"/>
+      <c r="CH9" s="12"/>
+      <c r="CI9" s="12"/>
+      <c r="CJ9" s="12"/>
+      <c r="CK9" s="12"/>
+      <c r="CL9" s="12"/>
+      <c r="CM9" s="12"/>
+      <c r="CN9" s="12"/>
+      <c r="CO9" s="12"/>
+      <c r="CP9" s="12"/>
+      <c r="CQ9" s="12"/>
+      <c r="CR9" s="12"/>
+      <c r="CS9" s="12"/>
+      <c r="CT9" s="12"/>
+      <c r="CU9" s="12"/>
+      <c r="CV9" s="12"/>
+      <c r="CW9" s="12"/>
+      <c r="CX9" s="12"/>
+    </row>
+    <row r="10" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="5"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+      <c r="AG10" s="7"/>
+      <c r="AH10" s="7"/>
+      <c r="AI10" s="7"/>
+      <c r="AJ10" s="7"/>
+      <c r="AK10" s="7"/>
+      <c r="AL10" s="7"/>
+      <c r="AM10" s="7"/>
+      <c r="AN10" s="7"/>
+      <c r="AO10" s="7"/>
+      <c r="AP10" s="7"/>
+      <c r="AQ10" s="7"/>
+      <c r="AR10" s="7"/>
+      <c r="AS10" s="6"/>
+      <c r="AT10" s="7"/>
+      <c r="AU10" s="7"/>
+      <c r="AV10" s="7"/>
+      <c r="AW10" s="7"/>
+      <c r="AX10" s="7"/>
+      <c r="AY10" s="7"/>
+      <c r="AZ10" s="7"/>
+      <c r="BA10" s="7"/>
+      <c r="BB10" s="7"/>
+      <c r="BC10" s="7"/>
+      <c r="BD10" s="7"/>
+      <c r="BE10" s="7"/>
+      <c r="BF10" s="6"/>
+      <c r="BG10" s="7"/>
+      <c r="BH10" s="7"/>
+      <c r="BI10" s="7"/>
+      <c r="BJ10" s="5"/>
+      <c r="BK10" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL10" s="12" t="n">
+        <v>8</v>
+      </c>
+      <c r="BM10" s="12"/>
+      <c r="BN10" s="12"/>
+      <c r="BO10" s="12"/>
+      <c r="BP10" s="12"/>
+      <c r="BQ10" s="12"/>
+      <c r="BR10" s="12"/>
+      <c r="BS10" s="12"/>
+      <c r="BT10" s="12"/>
+      <c r="BU10" s="12"/>
+      <c r="BV10" s="12"/>
+      <c r="BW10" s="12"/>
+      <c r="BX10" s="12"/>
+      <c r="BY10" s="12"/>
+      <c r="BZ10" s="12"/>
+      <c r="CA10" s="12"/>
+      <c r="CB10" s="12"/>
+      <c r="CC10" s="12"/>
+      <c r="CD10" s="12"/>
+      <c r="CE10" s="12"/>
+      <c r="CF10" s="12"/>
+      <c r="CG10" s="12"/>
+      <c r="CH10" s="12"/>
+      <c r="CI10" s="12"/>
+      <c r="CJ10" s="12"/>
+      <c r="CK10" s="12"/>
+      <c r="CL10" s="12"/>
+      <c r="CM10" s="12"/>
+      <c r="CN10" s="12"/>
+      <c r="CO10" s="12"/>
+      <c r="CP10" s="12"/>
+      <c r="CQ10" s="12"/>
+      <c r="CR10" s="12"/>
+      <c r="CS10" s="12"/>
+      <c r="CT10" s="12"/>
+      <c r="CU10" s="12"/>
+      <c r="CV10" s="12"/>
+      <c r="CW10" s="12"/>
+      <c r="CX10" s="12"/>
+    </row>
+    <row r="11" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="7"/>
+      <c r="M11" s="7"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="7"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="7"/>
+      <c r="AD11" s="7"/>
+      <c r="AE11" s="7"/>
+      <c r="AF11" s="7"/>
+      <c r="AG11" s="7"/>
+      <c r="AH11" s="7"/>
+      <c r="AI11" s="7"/>
+      <c r="AJ11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AK11" s="7"/>
+      <c r="AL11" s="7"/>
+      <c r="AM11" s="7"/>
+      <c r="AN11" s="7"/>
+      <c r="AO11" s="7"/>
+      <c r="AP11" s="7"/>
+      <c r="AQ11" s="7"/>
+      <c r="AR11" s="7"/>
+      <c r="AS11" s="6"/>
+      <c r="AT11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AU11" s="7"/>
+      <c r="AV11" s="7"/>
+      <c r="AW11" s="7"/>
+      <c r="AX11" s="7"/>
+      <c r="AY11" s="7"/>
+      <c r="AZ11" s="7"/>
+      <c r="BA11" s="7"/>
+      <c r="BB11" s="7"/>
+      <c r="BC11" s="7"/>
+      <c r="BD11" s="7"/>
+      <c r="BE11" s="7"/>
+      <c r="BF11" s="6"/>
+      <c r="BG11" s="7"/>
+      <c r="BH11" s="7"/>
+      <c r="BI11" s="7"/>
+      <c r="BJ11" s="5"/>
+      <c r="BK11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL11" s="12" t="n">
+        <v>9</v>
+      </c>
+      <c r="BM11" s="12"/>
+      <c r="BN11" s="12"/>
+      <c r="BO11" s="12"/>
+      <c r="BP11" s="12"/>
+      <c r="BQ11" s="12"/>
+      <c r="BR11" s="12"/>
+      <c r="BS11" s="12"/>
+      <c r="BT11" s="12"/>
+      <c r="BU11" s="12"/>
+      <c r="BV11" s="12"/>
+      <c r="BW11" s="12"/>
+      <c r="BX11" s="12"/>
+      <c r="BY11" s="12"/>
+      <c r="BZ11" s="12"/>
+      <c r="CA11" s="12"/>
+      <c r="CB11" s="12"/>
+      <c r="CC11" s="12"/>
+      <c r="CD11" s="12"/>
+      <c r="CE11" s="12"/>
+      <c r="CF11" s="12"/>
+      <c r="CG11" s="12"/>
+      <c r="CH11" s="12"/>
+      <c r="CI11" s="12"/>
+      <c r="CJ11" s="12"/>
+      <c r="CK11" s="12"/>
+      <c r="CL11" s="12"/>
+      <c r="CM11" s="12"/>
+      <c r="CN11" s="12"/>
+      <c r="CO11" s="12"/>
+      <c r="CP11" s="12"/>
+      <c r="CQ11" s="12"/>
+      <c r="CR11" s="12"/>
+      <c r="CS11" s="12"/>
+      <c r="CT11" s="12"/>
+      <c r="CU11" s="12"/>
+      <c r="CV11" s="12"/>
+      <c r="CW11" s="12"/>
+      <c r="CX11" s="12"/>
+    </row>
+    <row r="12" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
+      <c r="AB12" s="6"/>
+      <c r="AC12" s="7"/>
+      <c r="AD12" s="7"/>
+      <c r="AE12" s="7"/>
+      <c r="AF12" s="7"/>
+      <c r="AG12" s="7"/>
+      <c r="AH12" s="7"/>
+      <c r="AI12" s="7"/>
+      <c r="AJ12" s="7"/>
+      <c r="AK12" s="7"/>
+      <c r="AL12" s="7"/>
+      <c r="AM12" s="7"/>
+      <c r="AN12" s="7"/>
+      <c r="AO12" s="7"/>
+      <c r="AP12" s="7"/>
+      <c r="AQ12" s="7"/>
+      <c r="AR12" s="7"/>
+      <c r="AS12" s="6"/>
+      <c r="AT12" s="6"/>
+      <c r="AU12" s="6"/>
+      <c r="AV12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW12" s="6"/>
+      <c r="AX12" s="6"/>
+      <c r="AY12" s="6"/>
+      <c r="AZ12" s="6"/>
+      <c r="BA12" s="6"/>
+      <c r="BB12" s="6"/>
+      <c r="BC12" s="6"/>
+      <c r="BD12" s="6"/>
+      <c r="BE12" s="6"/>
+      <c r="BF12" s="6"/>
+      <c r="BG12" s="7"/>
+      <c r="BH12" s="7"/>
+      <c r="BI12" s="7"/>
+      <c r="BJ12" s="5"/>
+      <c r="BK12" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL12" s="12" t="n">
+        <v>10</v>
+      </c>
+      <c r="BM12" s="12"/>
+      <c r="BN12" s="12"/>
+      <c r="BO12" s="12"/>
+      <c r="BP12" s="12"/>
+      <c r="BQ12" s="12"/>
+      <c r="BR12" s="12"/>
+      <c r="BS12" s="12"/>
+      <c r="BT12" s="12"/>
+      <c r="BU12" s="12"/>
+      <c r="BV12" s="12"/>
+      <c r="BW12" s="12"/>
+      <c r="BX12" s="12"/>
+      <c r="BY12" s="12"/>
+      <c r="BZ12" s="12"/>
+      <c r="CA12" s="12"/>
+      <c r="CB12" s="12"/>
+      <c r="CC12" s="12"/>
+      <c r="CD12" s="12"/>
+      <c r="CE12" s="12"/>
+      <c r="CF12" s="12"/>
+      <c r="CG12" s="12"/>
+      <c r="CH12" s="12"/>
+      <c r="CI12" s="12"/>
+      <c r="CJ12" s="12"/>
+      <c r="CK12" s="12"/>
+      <c r="CL12" s="12"/>
+      <c r="CM12" s="12"/>
+      <c r="CN12" s="12"/>
+      <c r="CO12" s="12"/>
+      <c r="CP12" s="12"/>
+      <c r="CQ12" s="12"/>
+      <c r="CR12" s="12"/>
+      <c r="CS12" s="12"/>
+      <c r="CT12" s="12"/>
+      <c r="CU12" s="12"/>
+      <c r="CV12" s="12"/>
+      <c r="CW12" s="12"/>
+      <c r="CX12" s="12"/>
+    </row>
+    <row r="13" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
+      <c r="Q13" s="6"/>
+      <c r="R13" s="6"/>
+      <c r="S13" s="6"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+      <c r="AB13" s="6"/>
+      <c r="AC13" s="7"/>
+      <c r="AD13" s="7"/>
+      <c r="AE13" s="7"/>
+      <c r="AF13" s="7"/>
+      <c r="AG13" s="7"/>
+      <c r="AH13" s="7"/>
+      <c r="AI13" s="7"/>
+      <c r="AJ13" s="7"/>
+      <c r="AK13" s="7"/>
+      <c r="AL13" s="7"/>
+      <c r="AM13" s="7"/>
+      <c r="AN13" s="7"/>
+      <c r="AO13" s="7"/>
+      <c r="AP13" s="7"/>
+      <c r="AQ13" s="7"/>
+      <c r="AR13" s="7"/>
+      <c r="AS13" s="6"/>
+      <c r="AT13" s="8"/>
+      <c r="AU13" s="8"/>
+      <c r="AV13" s="7"/>
+      <c r="AW13" s="8"/>
+      <c r="AX13" s="8"/>
+      <c r="AY13" s="8"/>
+      <c r="AZ13" s="8"/>
+      <c r="BA13" s="8"/>
+      <c r="BB13" s="8"/>
+      <c r="BC13" s="8"/>
+      <c r="BD13" s="8"/>
+      <c r="BE13" s="8"/>
+      <c r="BF13" s="6"/>
+      <c r="BG13" s="7"/>
+      <c r="BH13" s="7"/>
+      <c r="BI13" s="7"/>
+      <c r="BJ13" s="5"/>
+      <c r="BK13" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL13" s="12" t="n">
+        <v>11</v>
+      </c>
+      <c r="BM13" s="12"/>
+      <c r="BN13" s="12"/>
+      <c r="BO13" s="12"/>
+      <c r="BP13" s="12"/>
+      <c r="BQ13" s="12"/>
+      <c r="BR13" s="12"/>
+      <c r="BS13" s="12"/>
+      <c r="BT13" s="12"/>
+      <c r="BU13" s="12"/>
+      <c r="BV13" s="12"/>
+      <c r="BW13" s="12"/>
+      <c r="BX13" s="12"/>
+      <c r="BY13" s="12"/>
+      <c r="BZ13" s="12"/>
+      <c r="CA13" s="12"/>
+      <c r="CB13" s="12"/>
+      <c r="CC13" s="12"/>
+      <c r="CD13" s="12"/>
+      <c r="CE13" s="12"/>
+      <c r="CF13" s="12"/>
+      <c r="CG13" s="12"/>
+      <c r="CH13" s="12"/>
+      <c r="CI13" s="12"/>
+      <c r="CJ13" s="12"/>
+      <c r="CK13" s="12"/>
+      <c r="CL13" s="12"/>
+      <c r="CM13" s="12"/>
+      <c r="CN13" s="12"/>
+      <c r="CO13" s="12"/>
+      <c r="CP13" s="12"/>
+      <c r="CQ13" s="12"/>
+      <c r="CR13" s="12"/>
+      <c r="CS13" s="12"/>
+      <c r="CT13" s="12"/>
+      <c r="CU13" s="12"/>
+      <c r="CV13" s="12"/>
+      <c r="CW13" s="12"/>
+      <c r="CX13" s="12"/>
+    </row>
+    <row r="14" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" s="5"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+      <c r="T14" s="8"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA14" s="7"/>
+      <c r="AB14" s="6"/>
+      <c r="AC14" s="7"/>
+      <c r="AD14" s="7"/>
+      <c r="AE14" s="7"/>
+      <c r="AF14" s="7"/>
+      <c r="AG14" s="7"/>
+      <c r="AH14" s="7"/>
+      <c r="AI14" s="7"/>
+      <c r="AJ14" s="7"/>
+      <c r="AK14" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL14" s="7"/>
+      <c r="AM14" s="7"/>
+      <c r="AN14" s="7"/>
+      <c r="AO14" s="7"/>
+      <c r="AP14" s="7"/>
+      <c r="AQ14" s="7"/>
+      <c r="AR14" s="7"/>
+      <c r="AS14" s="6"/>
+      <c r="AT14" s="7"/>
+      <c r="AU14" s="7"/>
+      <c r="AV14" s="7"/>
+      <c r="AW14" s="7"/>
+      <c r="AX14" s="7"/>
+      <c r="AY14" s="7"/>
+      <c r="AZ14" s="7"/>
+      <c r="BA14" s="7"/>
+      <c r="BB14" s="7"/>
+      <c r="BC14" s="7"/>
+      <c r="BD14" s="7"/>
+      <c r="BE14" s="7"/>
+      <c r="BF14" s="6"/>
+      <c r="BG14" s="7"/>
+      <c r="BH14" s="7"/>
+      <c r="BI14" s="7"/>
+      <c r="BJ14" s="5"/>
+      <c r="BK14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL14" s="12" t="n">
+        <v>12</v>
+      </c>
+      <c r="BM14" s="12"/>
+      <c r="BN14" s="12"/>
+      <c r="BO14" s="12"/>
+      <c r="BP14" s="12"/>
+      <c r="BQ14" s="12"/>
+      <c r="BR14" s="12"/>
+      <c r="BS14" s="12"/>
+      <c r="BT14" s="12"/>
+      <c r="BU14" s="12"/>
+      <c r="BV14" s="12"/>
+      <c r="BW14" s="12"/>
+      <c r="BX14" s="12"/>
+      <c r="BY14" s="12"/>
+      <c r="BZ14" s="12"/>
+      <c r="CA14" s="12"/>
+      <c r="CB14" s="12"/>
+      <c r="CC14" s="12"/>
+      <c r="CD14" s="12"/>
+      <c r="CE14" s="12"/>
+      <c r="CF14" s="12"/>
+      <c r="CG14" s="12"/>
+      <c r="CH14" s="12"/>
+      <c r="CI14" s="12"/>
+      <c r="CJ14" s="12"/>
+      <c r="CK14" s="12"/>
+      <c r="CL14" s="12"/>
+      <c r="CM14" s="12"/>
+      <c r="CN14" s="12"/>
+      <c r="CO14" s="12"/>
+      <c r="CP14" s="12"/>
+      <c r="CQ14" s="12"/>
+      <c r="CR14" s="12"/>
+      <c r="CS14" s="12"/>
+      <c r="CT14" s="12"/>
+      <c r="CU14" s="12"/>
+      <c r="CV14" s="12"/>
+      <c r="CW14" s="12"/>
+      <c r="CX14" s="12"/>
+    </row>
+    <row r="15" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" s="5"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="6"/>
+      <c r="AC15" s="7"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="7"/>
+      <c r="AH15" s="7"/>
+      <c r="AI15" s="7"/>
+      <c r="AJ15" s="7"/>
+      <c r="AK15" s="7"/>
+      <c r="AL15" s="7"/>
+      <c r="AM15" s="7"/>
+      <c r="AN15" s="7"/>
+      <c r="AO15" s="7"/>
+      <c r="AP15" s="7"/>
+      <c r="AQ15" s="7"/>
+      <c r="AR15" s="7"/>
+      <c r="AS15" s="6"/>
+      <c r="AT15" s="7"/>
+      <c r="AU15" s="7"/>
+      <c r="AV15" s="7"/>
+      <c r="AW15" s="7"/>
+      <c r="AX15" s="7"/>
+      <c r="AY15" s="7"/>
+      <c r="AZ15" s="7"/>
+      <c r="BA15" s="7"/>
+      <c r="BB15" s="7"/>
+      <c r="BC15" s="7"/>
+      <c r="BD15" s="7"/>
+      <c r="BE15" s="7"/>
+      <c r="BF15" s="6"/>
+      <c r="BG15" s="7"/>
+      <c r="BH15" s="7"/>
+      <c r="BI15" s="7"/>
+      <c r="BJ15" s="5"/>
+      <c r="BK15" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL15" s="12" t="n">
+        <v>13</v>
+      </c>
+      <c r="BM15" s="12"/>
+      <c r="BN15" s="12"/>
+      <c r="BO15" s="12"/>
+      <c r="BP15" s="12"/>
+      <c r="BQ15" s="12"/>
+      <c r="BR15" s="12"/>
+      <c r="BS15" s="12"/>
+      <c r="BT15" s="12"/>
+      <c r="BU15" s="12"/>
+      <c r="BV15" s="12"/>
+      <c r="BW15" s="12"/>
+      <c r="BX15" s="12"/>
+      <c r="BY15" s="12"/>
+      <c r="BZ15" s="12"/>
+      <c r="CA15" s="12"/>
+      <c r="CB15" s="12"/>
+      <c r="CC15" s="12"/>
+      <c r="CD15" s="12"/>
+      <c r="CE15" s="12"/>
+      <c r="CF15" s="12"/>
+      <c r="CG15" s="12"/>
+      <c r="CH15" s="12"/>
+      <c r="CI15" s="12"/>
+      <c r="CJ15" s="12"/>
+      <c r="CK15" s="12"/>
+      <c r="CL15" s="12"/>
+      <c r="CM15" s="12"/>
+      <c r="CN15" s="12"/>
+      <c r="CO15" s="12"/>
+      <c r="CP15" s="12"/>
+      <c r="CQ15" s="12"/>
+      <c r="CR15" s="12"/>
+      <c r="CS15" s="12"/>
+      <c r="CT15" s="12"/>
+      <c r="CU15" s="12"/>
+      <c r="CV15" s="12"/>
+      <c r="CW15" s="12"/>
+      <c r="CX15" s="12"/>
+    </row>
+    <row r="16" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" s="5"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
+      <c r="AB16" s="8"/>
+      <c r="AC16" s="7"/>
+      <c r="AD16" s="7"/>
+      <c r="AE16" s="7"/>
+      <c r="AF16" s="7"/>
+      <c r="AG16" s="7"/>
+      <c r="AH16" s="7"/>
+      <c r="AI16" s="7"/>
+      <c r="AJ16" s="7"/>
+      <c r="AK16" s="7"/>
+      <c r="AL16" s="7"/>
+      <c r="AM16" s="7"/>
+      <c r="AN16" s="7"/>
+      <c r="AO16" s="7"/>
+      <c r="AP16" s="7"/>
+      <c r="AQ16" s="7"/>
+      <c r="AR16" s="7"/>
+      <c r="AS16" s="6"/>
+      <c r="AT16" s="6"/>
+      <c r="AU16" s="6"/>
+      <c r="AV16" s="6"/>
+      <c r="AW16" s="6"/>
+      <c r="AX16" s="6"/>
+      <c r="AY16" s="6"/>
+      <c r="AZ16" s="6"/>
+      <c r="BA16" s="6"/>
+      <c r="BB16" s="6"/>
+      <c r="BC16" s="7"/>
+      <c r="BD16" s="7"/>
+      <c r="BE16" s="7"/>
+      <c r="BF16" s="6"/>
+      <c r="BG16" s="7"/>
+      <c r="BH16" s="7"/>
+      <c r="BI16" s="7"/>
+      <c r="BJ16" s="5"/>
+      <c r="BK16" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL16" s="12" t="n">
+        <v>14</v>
+      </c>
+      <c r="BM16" s="12"/>
+      <c r="BN16" s="12"/>
+      <c r="BO16" s="12"/>
+      <c r="BP16" s="12"/>
+      <c r="BQ16" s="12"/>
+      <c r="BR16" s="12"/>
+      <c r="BS16" s="12"/>
+      <c r="BT16" s="12"/>
+      <c r="BU16" s="12"/>
+      <c r="BV16" s="12"/>
+      <c r="BW16" s="12"/>
+      <c r="BX16" s="12"/>
+      <c r="BY16" s="12"/>
+      <c r="BZ16" s="12"/>
+      <c r="CA16" s="12"/>
+      <c r="CB16" s="12"/>
+      <c r="CC16" s="12"/>
+      <c r="CD16" s="12"/>
+      <c r="CE16" s="12"/>
+      <c r="CF16" s="12"/>
+      <c r="CG16" s="12"/>
+      <c r="CH16" s="12"/>
+      <c r="CI16" s="12"/>
+      <c r="CJ16" s="12"/>
+      <c r="CK16" s="12"/>
+      <c r="CL16" s="12"/>
+      <c r="CM16" s="12"/>
+      <c r="CN16" s="12"/>
+      <c r="CO16" s="12"/>
+      <c r="CP16" s="12"/>
+      <c r="CQ16" s="12"/>
+      <c r="CR16" s="12"/>
+      <c r="CS16" s="12"/>
+      <c r="CT16" s="12"/>
+      <c r="CU16" s="12"/>
+      <c r="CV16" s="12"/>
+      <c r="CW16" s="12"/>
+      <c r="CX16" s="12"/>
+    </row>
+    <row r="17" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
+      <c r="Q17" s="6"/>
+      <c r="R17" s="6"/>
+      <c r="S17" s="6"/>
+      <c r="T17" s="6"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AC17" s="7"/>
+      <c r="AD17" s="7"/>
+      <c r="AE17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="7"/>
+      <c r="AH17" s="7"/>
+      <c r="AI17" s="7"/>
+      <c r="AJ17" s="7"/>
+      <c r="AK17" s="7"/>
+      <c r="AL17" s="7"/>
+      <c r="AM17" s="7"/>
+      <c r="AN17" s="7"/>
+      <c r="AO17" s="7"/>
+      <c r="AP17" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ17" s="7"/>
+      <c r="AR17" s="7"/>
+      <c r="AS17" s="6"/>
+      <c r="AT17" s="8"/>
+      <c r="AU17" s="8"/>
+      <c r="AV17" s="8"/>
+      <c r="AW17" s="8"/>
+      <c r="AX17" s="8"/>
+      <c r="AY17" s="8"/>
+      <c r="AZ17" s="8"/>
+      <c r="BA17" s="8"/>
+      <c r="BB17" s="8"/>
+      <c r="BC17" s="7"/>
+      <c r="BD17" s="7"/>
+      <c r="BE17" s="7"/>
+      <c r="BF17" s="6"/>
+      <c r="BG17" s="7"/>
+      <c r="BH17" s="7"/>
+      <c r="BI17" s="7"/>
+      <c r="BJ17" s="5"/>
+      <c r="BK17" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL17" s="12" t="n">
+        <v>15</v>
+      </c>
+      <c r="BM17" s="12"/>
+      <c r="BN17" s="12"/>
+      <c r="BO17" s="12"/>
+      <c r="BP17" s="12"/>
+      <c r="BQ17" s="12"/>
+      <c r="BR17" s="12"/>
+      <c r="BS17" s="12"/>
+      <c r="BT17" s="12"/>
+      <c r="BU17" s="12"/>
+      <c r="BV17" s="12"/>
+      <c r="BW17" s="12"/>
+      <c r="BX17" s="12"/>
+      <c r="BY17" s="12"/>
+      <c r="BZ17" s="12"/>
+      <c r="CA17" s="12"/>
+      <c r="CB17" s="12"/>
+      <c r="CC17" s="12"/>
+      <c r="CD17" s="12"/>
+      <c r="CE17" s="12"/>
+      <c r="CF17" s="12"/>
+      <c r="CG17" s="12"/>
+      <c r="CH17" s="12"/>
+      <c r="CI17" s="12"/>
+      <c r="CJ17" s="12"/>
+      <c r="CK17" s="12"/>
+      <c r="CL17" s="12"/>
+      <c r="CM17" s="12"/>
+      <c r="CN17" s="12"/>
+      <c r="CO17" s="12"/>
+      <c r="CP17" s="12"/>
+      <c r="CQ17" s="12"/>
+      <c r="CR17" s="12"/>
+      <c r="CS17" s="12"/>
+      <c r="CT17" s="12"/>
+      <c r="CU17" s="12"/>
+      <c r="CV17" s="12"/>
+      <c r="CW17" s="12"/>
+      <c r="CX17" s="12"/>
+    </row>
+    <row r="18" spans="1:102" ht="23.70" customHeight="1">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" s="5"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+      <c r="M18" s="8"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="8"/>
+      <c r="P18" s="8"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+      <c r="T18" s="8"/>
+      <c r="U18" s="8"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
+      <c r="AB18" s="6"/>
+      <c r="AC18" s="7"/>
+      <c r="AD18" s="7"/>
+      <c r="AE18" s="6"/>
+      <c r="AF18" s="7"/>
+      <c r="AG18" s="7"/>
+      <c r="AH18" s="7"/>
+      <c r="AI18" s="6"/>
+      <c r="AJ18" s="6"/>
+      <c r="AK18" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="AL18" s="6"/>
+      <c r="AM18" s="6"/>
+      <c r="AN18" s="7"/>
+      <c r="AO18" s="7"/>
+      <c r="AP18" s="6"/>
+      <c r="AQ18" s="7"/>
+      <c r="AR18" s="7"/>
+      <c r="AS18" s="8"/>
+      <c r="AT18" s="7"/>
+      <c r="AU18" s="7"/>
+      <c r="AV18" s="7"/>
+      <c r="AW18" s="7"/>
+      <c r="AX18" s="7"/>
+      <c r="AY18" s="7"/>
+      <c r="AZ18" s="7"/>
+      <c r="BA18" s="7"/>
+      <c r="BB18" s="7"/>
+      <c r="BC18" s="7"/>
+      <c r="BD18" s="7"/>
+      <c r="BE18" s="7"/>
+      <c r="BF18" s="6"/>
+      <c r="BG18" s="7"/>
+      <c r="BH18" s="7"/>
+      <c r="BI18" s="7"/>
+      <c r="BJ18" s="5"/>
+      <c r="BK18" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL18" s="12" t="n">
+        <v>16</v>
+      </c>
+      <c r="BM18" s="12"/>
+      <c r="BN18" s="12"/>
+      <c r="BO18" s="12"/>
+      <c r="BP18" s="12"/>
+      <c r="BQ18" s="12"/>
+      <c r="BR18" s="12"/>
+      <c r="BS18" s="12"/>
+      <c r="BT18" s="12"/>
+      <c r="BU18" s="12"/>
+      <c r="BV18" s="12"/>
+      <c r="BW18" s="12"/>
+      <c r="BX18" s="12"/>
+      <c r="BY18" s="12"/>
+      <c r="BZ18" s="12"/>
+      <c r="CA18" s="12"/>
+      <c r="CB18" s="12"/>
+      <c r="CC18" s="12"/>
+      <c r="CD18" s="12"/>
+      <c r="CE18" s="12"/>
+      <c r="CF18" s="12"/>
+      <c r="CG18" s="12"/>
+      <c r="CH18" s="12"/>
+      <c r="CI18" s="12"/>
+      <c r="CJ18" s="12"/>
+      <c r="CK18" s="12"/>
+      <c r="CL18" s="12"/>
+      <c r="CM18" s="12"/>
+      <c r="CN18" s="12"/>
+      <c r="CO18" s="12"/>
+      <c r="CP18" s="12"/>
+      <c r="CQ18" s="12"/>
+      <c r="CR18" s="12"/>
+      <c r="CS18" s="12"/>
+      <c r="CT18" s="12"/>
+      <c r="CU18" s="12"/>
+      <c r="CV18" s="12"/>
+      <c r="CW18" s="12"/>
+      <c r="CX18" s="12"/>
+    </row>
+    <row r="19" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" s="5"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="6"/>
+      <c r="AC19" s="7"/>
+      <c r="AD19" s="7"/>
+      <c r="AE19" s="8"/>
+      <c r="AF19" s="7"/>
+      <c r="AG19" s="7"/>
+      <c r="AH19" s="7"/>
+      <c r="AI19" s="6"/>
+      <c r="AJ19" s="8"/>
+      <c r="AK19" s="7"/>
+      <c r="AL19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="AM19" s="6"/>
+      <c r="AN19" s="7"/>
+      <c r="AO19" s="7"/>
+      <c r="AP19" s="8"/>
+      <c r="AQ19" s="7"/>
+      <c r="AR19" s="7"/>
+      <c r="AS19" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT19" s="7"/>
+      <c r="AU19" s="7"/>
+      <c r="AV19" s="7"/>
+      <c r="AW19" s="7"/>
+      <c r="AX19" s="7"/>
+      <c r="AY19" s="7"/>
+      <c r="AZ19" s="7"/>
+      <c r="BA19" s="7"/>
+      <c r="BB19" s="7"/>
+      <c r="BC19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="BD19" s="7"/>
+      <c r="BE19" s="7"/>
+      <c r="BF19" s="6"/>
+      <c r="BG19" s="7"/>
+      <c r="BH19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="BI19" s="7"/>
+      <c r="BJ19" s="5"/>
+      <c r="BK19" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL19" s="12" t="n">
+        <v>17</v>
+      </c>
+      <c r="BM19" s="12"/>
+      <c r="BN19" s="12"/>
+      <c r="BO19" s="12"/>
+      <c r="BP19" s="12"/>
+      <c r="BQ19" s="12"/>
+      <c r="BR19" s="12"/>
+      <c r="BS19" s="12"/>
+      <c r="BT19" s="12"/>
+      <c r="BU19" s="12"/>
+      <c r="BV19" s="12"/>
+      <c r="BW19" s="12"/>
+      <c r="BX19" s="12"/>
+      <c r="BY19" s="12"/>
+      <c r="BZ19" s="12"/>
+      <c r="CA19" s="12"/>
+      <c r="CB19" s="12"/>
+      <c r="CC19" s="12"/>
+      <c r="CD19" s="12"/>
+      <c r="CE19" s="12"/>
+      <c r="CF19" s="12"/>
+      <c r="CG19" s="12"/>
+      <c r="CH19" s="12"/>
+      <c r="CI19" s="12"/>
+      <c r="CJ19" s="12"/>
+      <c r="CK19" s="12"/>
+      <c r="CL19" s="12"/>
+      <c r="CM19" s="12"/>
+      <c r="CN19" s="12"/>
+      <c r="CO19" s="12"/>
+      <c r="CP19" s="12"/>
+      <c r="CQ19" s="12"/>
+      <c r="CR19" s="12"/>
+      <c r="CS19" s="12"/>
+      <c r="CT19" s="12"/>
+      <c r="CU19" s="12"/>
+      <c r="CV19" s="12"/>
+      <c r="CW19" s="12"/>
+      <c r="CX19" s="12"/>
+    </row>
+    <row r="20" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="6"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
+      <c r="AB20" s="6"/>
+      <c r="AC20" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD20" s="7"/>
+      <c r="AE20" s="7"/>
+      <c r="AF20" s="7"/>
+      <c r="AG20" s="7"/>
+      <c r="AH20" s="7"/>
+      <c r="AI20" s="6"/>
+      <c r="AJ20" s="7"/>
+      <c r="AK20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL20" s="7"/>
+      <c r="AM20" s="6"/>
+      <c r="AN20" s="7"/>
+      <c r="AO20" s="7"/>
+      <c r="AP20" s="7"/>
+      <c r="AQ20" s="7"/>
+      <c r="AR20" s="7"/>
+      <c r="AS20" s="6"/>
+      <c r="AT20" s="7"/>
+      <c r="AU20" s="7"/>
+      <c r="AV20" s="7"/>
+      <c r="AW20" s="7"/>
+      <c r="AX20" s="7"/>
+      <c r="AY20" s="7"/>
+      <c r="AZ20" s="7"/>
+      <c r="BA20" s="7"/>
+      <c r="BB20" s="7"/>
+      <c r="BC20" s="7"/>
+      <c r="BD20" s="7"/>
+      <c r="BE20" s="7"/>
+      <c r="BF20" s="6"/>
+      <c r="BG20" s="7"/>
+      <c r="BH20" s="7"/>
+      <c r="BI20" s="7"/>
+      <c r="BJ20" s="5"/>
+      <c r="BK20" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL20" s="12" t="n">
+        <v>18</v>
+      </c>
+      <c r="BM20" s="12"/>
+      <c r="BN20" s="12"/>
+      <c r="BO20" s="12"/>
+      <c r="BP20" s="12"/>
+      <c r="BQ20" s="12"/>
+      <c r="BR20" s="12"/>
+      <c r="BS20" s="12"/>
+      <c r="BT20" s="12"/>
+      <c r="BU20" s="12"/>
+      <c r="BV20" s="12"/>
+      <c r="BW20" s="12"/>
+      <c r="BX20" s="12"/>
+      <c r="BY20" s="12"/>
+      <c r="BZ20" s="12"/>
+      <c r="CA20" s="12"/>
+      <c r="CB20" s="12"/>
+      <c r="CC20" s="12"/>
+      <c r="CD20" s="12"/>
+      <c r="CE20" s="12"/>
+      <c r="CF20" s="12"/>
+      <c r="CG20" s="12"/>
+      <c r="CH20" s="12"/>
+      <c r="CI20" s="12"/>
+      <c r="CJ20" s="12"/>
+      <c r="CK20" s="12"/>
+      <c r="CL20" s="12"/>
+      <c r="CM20" s="12"/>
+      <c r="CN20" s="12"/>
+      <c r="CO20" s="12"/>
+      <c r="CP20" s="12"/>
+      <c r="CQ20" s="12"/>
+      <c r="CR20" s="12"/>
+      <c r="CS20" s="12"/>
+      <c r="CT20" s="12"/>
+      <c r="CU20" s="12"/>
+      <c r="CV20" s="12"/>
+      <c r="CW20" s="12"/>
+      <c r="CX20" s="12"/>
+    </row>
+    <row r="21" spans="1:102" ht="23.85" customHeight="1">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5"/>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5"/>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+      <c r="W21" s="5"/>
+      <c r="X21" s="5"/>
+      <c r="Y21" s="5"/>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="5"/>
+      <c r="AB21" s="5"/>
+      <c r="AC21" s="5"/>
+      <c r="AD21" s="5"/>
+      <c r="AE21" s="5"/>
+      <c r="AF21" s="5"/>
+      <c r="AG21" s="5"/>
+      <c r="AH21" s="5"/>
+      <c r="AI21" s="5"/>
+      <c r="AJ21" s="5"/>
+      <c r="AK21" s="5"/>
+      <c r="AL21" s="5"/>
+      <c r="AM21" s="5"/>
+      <c r="AN21" s="5"/>
+      <c r="AO21" s="5"/>
+      <c r="AP21" s="10"/>
+      <c r="AQ21" s="10"/>
+      <c r="AR21" s="10"/>
+      <c r="AS21" s="10"/>
+      <c r="AT21" s="10"/>
+      <c r="AU21" s="10"/>
+      <c r="AV21" s="10"/>
+      <c r="AW21" s="10"/>
+      <c r="AX21" s="10"/>
+      <c r="AY21" s="10"/>
+      <c r="AZ21" s="10"/>
+      <c r="BA21" s="10"/>
+      <c r="BB21" s="10"/>
+      <c r="BC21" s="10"/>
+      <c r="BD21" s="10"/>
+      <c r="BE21" s="10"/>
+      <c r="BF21" s="10"/>
+      <c r="BG21" s="10"/>
+      <c r="BH21" s="10"/>
+      <c r="BI21" s="10"/>
+      <c r="BJ21" s="5"/>
+      <c r="BK21" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BL21" s="12" t="n">
+        <v>19</v>
+      </c>
+      <c r="BM21" s="12"/>
+      <c r="BN21" s="12"/>
+      <c r="BO21" s="12"/>
+      <c r="BP21" s="12"/>
+      <c r="BQ21" s="12"/>
+      <c r="BR21" s="12"/>
+      <c r="BS21" s="12"/>
+      <c r="BT21" s="12"/>
+      <c r="BU21" s="12"/>
+      <c r="BV21" s="12"/>
+      <c r="BW21" s="12"/>
+      <c r="BX21" s="12"/>
+      <c r="BY21" s="12"/>
+      <c r="BZ21" s="12"/>
+      <c r="CA21" s="12"/>
+      <c r="CB21" s="12"/>
+      <c r="CC21" s="12"/>
+      <c r="CD21" s="12"/>
+      <c r="CE21" s="12"/>
+      <c r="CF21" s="12"/>
+      <c r="CG21" s="12"/>
+      <c r="CH21" s="12"/>
+      <c r="CI21" s="12"/>
+      <c r="CJ21" s="12"/>
+      <c r="CK21" s="12"/>
+      <c r="CL21" s="12"/>
+      <c r="CM21" s="12"/>
+      <c r="CN21" s="12"/>
+      <c r="CO21" s="12"/>
+      <c r="CP21" s="12"/>
+      <c r="CQ21" s="12"/>
+      <c r="CR21" s="12"/>
+      <c r="CS21" s="12"/>
+      <c r="CT21" s="12"/>
+      <c r="CU21" s="12"/>
+      <c r="CV21" s="12"/>
+      <c r="CW21" s="12"/>
+      <c r="CX21" s="12"/>
+    </row>
+    <row r="22" spans="2:71">
+      <c r="B22" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+      <c r="S22" s="13"/>
+      <c r="X22" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y22" s="18"/>
+      <c r="Z22" s="18"/>
+      <c r="AA22" s="18"/>
+      <c r="AB22" s="18"/>
+      <c r="AC22" s="18"/>
+      <c r="AD22" s="18"/>
+      <c r="AE22" s="18"/>
+      <c r="AF22" s="18"/>
+      <c r="AG22" s="18"/>
+      <c r="AH22" s="18"/>
+      <c r="AI22" s="18"/>
+      <c r="AJ22" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="AK22" s="18"/>
+      <c r="AL22" s="18"/>
+      <c r="AM22" s="18"/>
+      <c r="AN22" s="18"/>
+      <c r="AO22" s="18"/>
+      <c r="AP22" s="18"/>
+      <c r="AQ22" s="18"/>
+      <c r="AR22" s="18"/>
+      <c r="AS22" s="18"/>
+      <c r="AT22" s="18"/>
+      <c r="AU22" s="18"/>
+      <c r="AV22" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="AW22" s="18"/>
+      <c r="AX22" s="18"/>
+      <c r="AY22" s="18"/>
+      <c r="AZ22" s="18"/>
+      <c r="BA22" s="18"/>
+      <c r="BB22" s="18"/>
+      <c r="BC22" s="18"/>
+      <c r="BD22" s="18"/>
+      <c r="BE22" s="18"/>
+      <c r="BF22" s="18"/>
+      <c r="BG22" s="18"/>
+      <c r="BH22" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="BI22" s="18"/>
+      <c r="BJ22" s="18"/>
+      <c r="BK22" s="18"/>
+      <c r="BL22" s="18"/>
+      <c r="BM22" s="18"/>
+      <c r="BN22" s="18"/>
+      <c r="BO22" s="18"/>
+      <c r="BP22" s="18"/>
+      <c r="BQ22" s="18"/>
+      <c r="BR22" s="18"/>
+      <c r="BS22" s="18"/>
+    </row>
+    <row r="23" spans="2:71">
+      <c r="B23" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="M23" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="13"/>
+      <c r="X23" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y23" s="18"/>
+      <c r="Z23" s="18"/>
+      <c r="AA23" s="18"/>
+      <c r="AB23" s="18"/>
+      <c r="AC23" s="18"/>
+      <c r="AD23" s="18"/>
+      <c r="AE23" s="18"/>
+      <c r="AF23" s="18"/>
+      <c r="AG23" s="18"/>
+      <c r="AH23" s="18"/>
+      <c r="AI23" s="18"/>
+      <c r="AJ23" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK23" s="18"/>
+      <c r="AL23" s="18"/>
+      <c r="AM23" s="18"/>
+      <c r="AN23" s="18"/>
+      <c r="AO23" s="18"/>
+      <c r="AP23" s="18"/>
+      <c r="AQ23" s="18"/>
+      <c r="AR23" s="18"/>
+      <c r="AS23" s="18"/>
+      <c r="AT23" s="18"/>
+      <c r="AU23" s="18"/>
+      <c r="AV23" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW23" s="18"/>
+      <c r="AX23" s="18"/>
+      <c r="AY23" s="18"/>
+      <c r="AZ23" s="18"/>
+      <c r="BA23" s="18"/>
+      <c r="BB23" s="18"/>
+      <c r="BC23" s="18"/>
+      <c r="BD23" s="18"/>
+      <c r="BE23" s="18"/>
+      <c r="BF23" s="18"/>
+      <c r="BG23" s="18"/>
+      <c r="BH23" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="BI23" s="18"/>
+      <c r="BJ23" s="18"/>
+      <c r="BK23" s="18"/>
+      <c r="BL23" s="18"/>
+      <c r="BM23" s="18"/>
+      <c r="BN23" s="18"/>
+      <c r="BO23" s="18"/>
+      <c r="BP23" s="18"/>
+      <c r="BQ23" s="18"/>
+      <c r="BR23" s="18"/>
+      <c r="BS23" s="18"/>
+    </row>
+    <row r="24" spans="2:71">
+      <c r="B24" s="15"/>
+      <c r="C24" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="X24" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y24" s="18"/>
+      <c r="Z24" s="18"/>
+      <c r="AA24" s="18"/>
+      <c r="AB24" s="18"/>
+      <c r="AC24" s="18"/>
+      <c r="AD24" s="18"/>
+      <c r="AE24" s="18"/>
+      <c r="AF24" s="18"/>
+      <c r="AG24" s="18"/>
+      <c r="AH24" s="18"/>
+      <c r="AI24" s="18"/>
+      <c r="AJ24" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK24" s="18"/>
+      <c r="AL24" s="18"/>
+      <c r="AM24" s="18"/>
+      <c r="AN24" s="18"/>
+      <c r="AO24" s="18"/>
+      <c r="AP24" s="18"/>
+      <c r="AQ24" s="18"/>
+      <c r="AR24" s="18"/>
+      <c r="AS24" s="18"/>
+      <c r="AT24" s="18"/>
+      <c r="AU24" s="18"/>
+      <c r="AV24" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="AW24" s="18"/>
+      <c r="AX24" s="18"/>
+      <c r="AY24" s="18"/>
+      <c r="AZ24" s="18"/>
+      <c r="BA24" s="18"/>
+      <c r="BB24" s="18"/>
+      <c r="BC24" s="18"/>
+      <c r="BD24" s="18"/>
+      <c r="BE24" s="18"/>
+      <c r="BF24" s="18"/>
+      <c r="BG24" s="18"/>
+      <c r="BH24" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="BI24" s="18"/>
+      <c r="BJ24" s="18"/>
+      <c r="BK24" s="18"/>
+      <c r="BL24" s="18"/>
+      <c r="BM24" s="18"/>
+      <c r="BN24" s="18"/>
+      <c r="BO24" s="18"/>
+      <c r="BP24" s="18"/>
+      <c r="BQ24" s="18"/>
+      <c r="BR24" s="18"/>
+      <c r="BS24" s="18"/>
+    </row>
+    <row r="25" spans="2:71">
+      <c r="B25" s="16"/>
+      <c r="C25" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="M25" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="X25" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y25" s="18"/>
+      <c r="Z25" s="18"/>
+      <c r="AA25" s="18"/>
+      <c r="AB25" s="18"/>
+      <c r="AC25" s="18"/>
+      <c r="AD25" s="18"/>
+      <c r="AE25" s="18"/>
+      <c r="AF25" s="18"/>
+      <c r="AG25" s="18"/>
+      <c r="AH25" s="18"/>
+      <c r="AI25" s="18"/>
+      <c r="AJ25" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="AK25" s="18"/>
+      <c r="AL25" s="18"/>
+      <c r="AM25" s="18"/>
+      <c r="AN25" s="18"/>
+      <c r="AO25" s="18"/>
+      <c r="AP25" s="18"/>
+      <c r="AQ25" s="18"/>
+      <c r="AR25" s="18"/>
+      <c r="AS25" s="18"/>
+      <c r="AT25" s="18"/>
+      <c r="AU25" s="18"/>
+      <c r="AV25" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="AW25" s="18"/>
+      <c r="AX25" s="18"/>
+      <c r="AY25" s="18"/>
+      <c r="AZ25" s="18"/>
+      <c r="BA25" s="18"/>
+      <c r="BB25" s="18"/>
+      <c r="BC25" s="18"/>
+      <c r="BD25" s="18"/>
+      <c r="BE25" s="18"/>
+      <c r="BF25" s="18"/>
+      <c r="BG25" s="18"/>
+      <c r="BH25" s="18"/>
+      <c r="BI25" s="18"/>
+      <c r="BJ25" s="18"/>
+      <c r="BK25" s="18"/>
+      <c r="BL25" s="18"/>
+      <c r="BM25" s="18"/>
+      <c r="BN25" s="18"/>
+      <c r="BO25" s="18"/>
+      <c r="BP25" s="18"/>
+      <c r="BQ25" s="18"/>
+      <c r="BR25" s="18"/>
+      <c r="BS25" s="18"/>
+    </row>
+    <row r="26" spans="2:71">
+      <c r="B26" s="17"/>
+      <c r="C26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="M26" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="X26" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y26" s="18"/>
+      <c r="Z26" s="18"/>
+      <c r="AA26" s="18"/>
+      <c r="AB26" s="18"/>
+      <c r="AC26" s="18"/>
+      <c r="AD26" s="18"/>
+      <c r="AE26" s="18"/>
+      <c r="AF26" s="18"/>
+      <c r="AG26" s="18"/>
+      <c r="AH26" s="18"/>
+      <c r="AI26" s="18"/>
+      <c r="AJ26" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="AK26" s="18"/>
+      <c r="AL26" s="18"/>
+      <c r="AM26" s="18"/>
+      <c r="AN26" s="18"/>
+      <c r="AO26" s="18"/>
+      <c r="AP26" s="18"/>
+      <c r="AQ26" s="18"/>
+      <c r="AR26" s="18"/>
+      <c r="AS26" s="18"/>
+      <c r="AT26" s="18"/>
+      <c r="AU26" s="18"/>
+      <c r="AV26" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="AW26" s="18"/>
+      <c r="AX26" s="18"/>
+      <c r="AY26" s="18"/>
+      <c r="AZ26" s="18"/>
+      <c r="BA26" s="18"/>
+      <c r="BB26" s="18"/>
+      <c r="BC26" s="18"/>
+      <c r="BD26" s="18"/>
+      <c r="BE26" s="18"/>
+      <c r="BF26" s="18"/>
+      <c r="BG26" s="18"/>
+      <c r="BH26" s="18"/>
+      <c r="BI26" s="18"/>
+      <c r="BJ26" s="18"/>
+      <c r="BK26" s="18"/>
+      <c r="BL26" s="18"/>
+      <c r="BM26" s="18"/>
+      <c r="BN26" s="18"/>
+      <c r="BO26" s="18"/>
+      <c r="BP26" s="18"/>
+      <c r="BQ26" s="18"/>
+      <c r="BR26" s="18"/>
+      <c r="BS26" s="18"/>
+    </row>
+    <row r="27" spans="2:71">
+      <c r="B27" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="M27" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="X27" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y27" s="18"/>
+      <c r="Z27" s="18"/>
+      <c r="AA27" s="18"/>
+      <c r="AB27" s="18"/>
+      <c r="AC27" s="18"/>
+      <c r="AD27" s="18"/>
+      <c r="AE27" s="18"/>
+      <c r="AF27" s="18"/>
+      <c r="AG27" s="18"/>
+      <c r="AH27" s="18"/>
+      <c r="AI27" s="18"/>
+      <c r="AJ27" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK27" s="18"/>
+      <c r="AL27" s="18"/>
+      <c r="AM27" s="18"/>
+      <c r="AN27" s="18"/>
+      <c r="AO27" s="18"/>
+      <c r="AP27" s="18"/>
+      <c r="AQ27" s="18"/>
+      <c r="AR27" s="18"/>
+      <c r="AS27" s="18"/>
+      <c r="AT27" s="18"/>
+      <c r="AU27" s="18"/>
+      <c r="AV27" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="AW27" s="18"/>
+      <c r="AX27" s="18"/>
+      <c r="AY27" s="18"/>
+      <c r="AZ27" s="18"/>
+      <c r="BA27" s="18"/>
+      <c r="BB27" s="18"/>
+      <c r="BC27" s="18"/>
+      <c r="BD27" s="18"/>
+      <c r="BE27" s="18"/>
+      <c r="BF27" s="18"/>
+      <c r="BG27" s="18"/>
+      <c r="BH27" s="18"/>
+      <c r="BI27" s="18"/>
+      <c r="BJ27" s="18"/>
+      <c r="BK27" s="18"/>
+      <c r="BL27" s="18"/>
+      <c r="BM27" s="18"/>
+      <c r="BN27" s="18"/>
+      <c r="BO27" s="18"/>
+      <c r="BP27" s="18"/>
+      <c r="BQ27" s="18"/>
+      <c r="BR27" s="18"/>
+      <c r="BS27" s="18"/>
+    </row>
+    <row r="28" spans="2:71">
+      <c r="B28" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+      <c r="L28" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="M28" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="X28" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y28" s="18"/>
+      <c r="Z28" s="18"/>
+      <c r="AA28" s="18"/>
+      <c r="AB28" s="18"/>
+      <c r="AC28" s="18"/>
+      <c r="AD28" s="18"/>
+      <c r="AE28" s="18"/>
+      <c r="AF28" s="18"/>
+      <c r="AG28" s="18"/>
+      <c r="AH28" s="18"/>
+      <c r="AI28" s="18"/>
+      <c r="AJ28" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK28" s="18"/>
+      <c r="AL28" s="18"/>
+      <c r="AM28" s="18"/>
+      <c r="AN28" s="18"/>
+      <c r="AO28" s="18"/>
+      <c r="AP28" s="18"/>
+      <c r="AQ28" s="18"/>
+      <c r="AR28" s="18"/>
+      <c r="AS28" s="18"/>
+      <c r="AT28" s="18"/>
+      <c r="AU28" s="18"/>
+      <c r="AV28" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="AW28" s="18"/>
+      <c r="AX28" s="18"/>
+      <c r="AY28" s="18"/>
+      <c r="AZ28" s="18"/>
+      <c r="BA28" s="18"/>
+      <c r="BB28" s="18"/>
+      <c r="BC28" s="18"/>
+      <c r="BD28" s="18"/>
+      <c r="BE28" s="18"/>
+      <c r="BF28" s="18"/>
+      <c r="BG28" s="18"/>
+      <c r="BH28" s="18"/>
+      <c r="BI28" s="18"/>
+      <c r="BJ28" s="18"/>
+      <c r="BK28" s="18"/>
+      <c r="BL28" s="18"/>
+      <c r="BM28" s="18"/>
+      <c r="BN28" s="18"/>
+      <c r="BO28" s="18"/>
+      <c r="BP28" s="18"/>
+      <c r="BQ28" s="18"/>
+      <c r="BR28" s="18"/>
+      <c r="BS28" s="18"/>
+    </row>
+    <row r="29" spans="2:71">
+      <c r="B29" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13"/>
+      <c r="M29" s="13"/>
+      <c r="N29" s="13"/>
+      <c r="O29" s="13"/>
+      <c r="P29" s="13"/>
+      <c r="Q29" s="13"/>
+      <c r="R29" s="13"/>
+      <c r="S29" s="13"/>
+      <c r="X29" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y29" s="18"/>
+      <c r="Z29" s="18"/>
+      <c r="AA29" s="18"/>
+      <c r="AB29" s="18"/>
+      <c r="AC29" s="18"/>
+      <c r="AD29" s="18"/>
+      <c r="AE29" s="18"/>
+      <c r="AF29" s="18"/>
+      <c r="AG29" s="18"/>
+      <c r="AH29" s="18"/>
+      <c r="AI29" s="18"/>
+      <c r="AJ29" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK29" s="18"/>
+      <c r="AL29" s="18"/>
+      <c r="AM29" s="18"/>
+      <c r="AN29" s="18"/>
+      <c r="AO29" s="18"/>
+      <c r="AP29" s="18"/>
+      <c r="AQ29" s="18"/>
+      <c r="AR29" s="18"/>
+      <c r="AS29" s="18"/>
+      <c r="AT29" s="18"/>
+      <c r="AU29" s="18"/>
+      <c r="AV29" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="AW29" s="18"/>
+      <c r="AX29" s="18"/>
+      <c r="AY29" s="18"/>
+      <c r="AZ29" s="18"/>
+      <c r="BA29" s="18"/>
+      <c r="BB29" s="18"/>
+      <c r="BC29" s="18"/>
+      <c r="BD29" s="18"/>
+      <c r="BE29" s="18"/>
+      <c r="BF29" s="18"/>
+      <c r="BG29" s="18"/>
+      <c r="BH29" s="18"/>
+      <c r="BI29" s="18"/>
+      <c r="BJ29" s="18"/>
+      <c r="BK29" s="18"/>
+      <c r="BL29" s="18"/>
+      <c r="BM29" s="18"/>
+      <c r="BN29" s="18"/>
+      <c r="BO29" s="18"/>
+      <c r="BP29" s="18"/>
+      <c r="BQ29" s="18"/>
+      <c r="BR29" s="18"/>
+      <c r="BS29" s="18"/>
+    </row>
+    <row r="30" spans="2:71">
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+      <c r="L30" s="13"/>
+      <c r="M30" s="13"/>
+      <c r="N30" s="13"/>
+      <c r="O30" s="13"/>
+      <c r="P30" s="13"/>
+      <c r="Q30" s="13"/>
+      <c r="R30" s="13"/>
+      <c r="S30" s="13"/>
+      <c r="X30" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y30" s="18"/>
+      <c r="Z30" s="18"/>
+      <c r="AA30" s="18"/>
+      <c r="AB30" s="18"/>
+      <c r="AC30" s="18"/>
+      <c r="AD30" s="18"/>
+      <c r="AE30" s="18"/>
+      <c r="AF30" s="18"/>
+      <c r="AG30" s="18"/>
+      <c r="AH30" s="18"/>
+      <c r="AI30" s="18"/>
+      <c r="AJ30" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="AK30" s="18"/>
+      <c r="AL30" s="18"/>
+      <c r="AM30" s="18"/>
+      <c r="AN30" s="18"/>
+      <c r="AO30" s="18"/>
+      <c r="AP30" s="18"/>
+      <c r="AQ30" s="18"/>
+      <c r="AR30" s="18"/>
+      <c r="AS30" s="18"/>
+      <c r="AT30" s="18"/>
+      <c r="AU30" s="18"/>
+      <c r="AV30" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="AW30" s="18"/>
+      <c r="AX30" s="18"/>
+      <c r="AY30" s="18"/>
+      <c r="AZ30" s="18"/>
+      <c r="BA30" s="18"/>
+      <c r="BB30" s="18"/>
+      <c r="BC30" s="18"/>
+      <c r="BD30" s="18"/>
+      <c r="BE30" s="18"/>
+      <c r="BF30" s="18"/>
+      <c r="BG30" s="18"/>
+      <c r="BH30" s="18"/>
+      <c r="BI30" s="18"/>
+      <c r="BJ30" s="18"/>
+      <c r="BK30" s="18"/>
+      <c r="BL30" s="18"/>
+      <c r="BM30" s="18"/>
+      <c r="BN30" s="18"/>
+      <c r="BO30" s="18"/>
+      <c r="BP30" s="18"/>
+      <c r="BQ30" s="18"/>
+      <c r="BR30" s="18"/>
+      <c r="BS30" s="18"/>
+    </row>
+    <row r="31" spans="3:3">
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="3:50">
+      <c r="C32" s="9"/>
+      <c r="AX32" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3">
+      <c r="C33" s="9"/>
+    </row>
+    <row r="34" spans="3:3">
+      <c r="C34" s="9"/>
+    </row>
+    <row r="35" spans="3:3">
+      <c r="C35" s="9"/>
+    </row>
+    <row r="36" spans="3:3">
+      <c r="C36" s="9"/>
+    </row>
+    <row r="37" spans="3:3">
+      <c r="C37" s="9"/>
+    </row>
+    <row r="38" spans="3:3">
+      <c r="C38" s="9"/>
+    </row>
+    <row r="39" spans="3:3">
+      <c r="C39" s="9"/>
+    </row>
+    <row r="40" spans="3:3">
+      <c r="C40" s="9"/>
+    </row>
+    <row r="41" spans="3:3">
+      <c r="C41" s="9"/>
+    </row>
+    <row r="42" spans="3:3">
+      <c r="C42" s="9"/>
+    </row>
+    <row r="43" spans="3:3">
+      <c r="C43" s="9"/>
+    </row>
+    <row r="44" spans="3:3">
+      <c r="C44" s="9"/>
+    </row>
+    <row r="45" spans="3:3">
+      <c r="C45" s="9"/>
+    </row>
+    <row r="46" spans="3:3">
+      <c r="C46" s="9"/>
+    </row>
+    <row r="47" spans="3:3">
+      <c r="C47" s="9"/>
+    </row>
+    <row r="48" spans="3:3">
+      <c r="C48" s="9"/>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" s="9"/>
+    </row>
+    <row r="50" spans="3:3">
+      <c r="C50" s="9"/>
+    </row>
+    <row r="51" spans="3:3">
+      <c r="C51" s="9"/>
+    </row>
+    <row r="52" spans="3:3">
+      <c r="C52" s="9"/>
+    </row>
+    <row r="53" spans="3:3">
+      <c r="C53" s="9"/>
+    </row>
+    <row r="54" spans="3:3">
+      <c r="C54" s="9"/>
+    </row>
+    <row r="55" spans="3:3">
+      <c r="C55" s="9"/>
+    </row>
+    <row r="56" spans="3:3">
+      <c r="C56" s="9"/>
+    </row>
+    <row r="57" spans="3:3">
+      <c r="C57" s="9"/>
+    </row>
+    <row r="58" spans="3:3">
+      <c r="C58" s="9"/>
+    </row>
+    <row r="59" spans="3:3">
+      <c r="C59" s="9"/>
+    </row>
+    <row r="60" spans="3:3">
+      <c r="C60" s="9"/>
+    </row>
+    <row r="61" spans="3:3">
+      <c r="C61" s="9"/>
+    </row>
+    <row r="62" spans="3:3">
+      <c r="C62" s="9"/>
+    </row>
+    <row r="63" spans="3:3">
+      <c r="C63" s="9"/>
+    </row>
+    <row r="64" spans="3:3">
+      <c r="C64" s="9"/>
+    </row>
+    <row r="65" spans="3:3">
+      <c r="C65" s="9"/>
+    </row>
+  </sheetData>
+  <mergeCells count="36">
+    <mergeCell ref="X22:AI22"/>
+    <mergeCell ref="AJ22:AU22"/>
+    <mergeCell ref="AV22:BG22"/>
+    <mergeCell ref="BH22:BS22"/>
+    <mergeCell ref="X23:AI23"/>
+    <mergeCell ref="AJ23:AU23"/>
+    <mergeCell ref="AV23:BG23"/>
+    <mergeCell ref="BH23:BS23"/>
+    <mergeCell ref="X24:AI24"/>
+    <mergeCell ref="AJ24:AU24"/>
+    <mergeCell ref="AV24:BG24"/>
+    <mergeCell ref="BH24:BS24"/>
+    <mergeCell ref="X25:AI25"/>
+    <mergeCell ref="AJ25:AU25"/>
+    <mergeCell ref="AV25:BG25"/>
+    <mergeCell ref="BH25:BS25"/>
+    <mergeCell ref="X26:AI26"/>
+    <mergeCell ref="AJ26:AU26"/>
+    <mergeCell ref="AV26:BG26"/>
+    <mergeCell ref="BH26:BS26"/>
+    <mergeCell ref="X27:AI27"/>
+    <mergeCell ref="AJ27:AU27"/>
+    <mergeCell ref="AV27:BG27"/>
+    <mergeCell ref="BH27:BS27"/>
+    <mergeCell ref="X28:AI28"/>
+    <mergeCell ref="AJ28:AU28"/>
+    <mergeCell ref="AV28:BG28"/>
+    <mergeCell ref="BH28:BS28"/>
+    <mergeCell ref="X29:AI29"/>
+    <mergeCell ref="AJ29:AU29"/>
+    <mergeCell ref="AV29:BG29"/>
+    <mergeCell ref="BH29:BS29"/>
+    <mergeCell ref="X30:AI30"/>
+    <mergeCell ref="AJ30:AU30"/>
+    <mergeCell ref="AV30:BG30"/>
+    <mergeCell ref="BH30:BS30"/>
+  </mergeCells>
+  <printOptions>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:pageFlags xmlns:pm="smNativeData" id="1586327817" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+      </ext>
+    </extLst>
+  </printOptions>
+  <pageMargins left="0.252083" right="0.252083" top="0.752083" bottom="0.752083" header="0.299306" footer="0.299306"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="1" pageOrder="overThenDown" orientation="landscape"/>
+  <headerFooter>
+    <extLst>
+      <ext uri="smNativeData">
+        <pm:header xmlns:pm="smNativeData" id="1586327817" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1586327817" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1586327817" Id="0" type="0" value="0"/>
+        <pm:paperBin xmlns:pm="smNativeData" id="1586327817" Id="1" type="0" value="0"/>
+      </ext>
+    </extLst>
+  </headerFooter>
+  <extLst>
+    <ext uri="smNativeData">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1586327817" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>